<commit_message>
quick little reinstall for scikit I am doing
</commit_message>
<xml_diff>
--- a/Players_Data.xlsx
+++ b/Players_Data.xlsx
@@ -184,7 +184,7 @@
     <t>Ariel Hukporti</t>
   </si>
   <si>
-    <t>Armel Traoré</t>
+    <t>Armel Traore</t>
   </si>
   <si>
     <t>Ausar Thompson</t>
@@ -1210,7 +1210,7 @@
     <t>Mouhamed Gueye</t>
   </si>
   <si>
-    <t>Moussa Diabaté</t>
+    <t>Moussa Diabate</t>
   </si>
   <si>
     <t>Myles Turner</t>
@@ -1483,7 +1483,7 @@
     <t>Taylor Hendricks</t>
   </si>
   <si>
-    <t>Tazé Moore</t>
+    <t>Taze Moore</t>
   </si>
   <si>
     <t>Terance Mann</t>
@@ -3590,34 +3590,34 @@
         <v>877</v>
       </c>
       <c r="O6">
+        <v>29</v>
+      </c>
+      <c r="P6">
+        <v>111</v>
+      </c>
+      <c r="Q6">
         <v>28</v>
       </c>
-      <c r="P6">
-        <v>105</v>
-      </c>
-      <c r="Q6">
-        <v>25</v>
-      </c>
       <c r="R6">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S6">
-        <v>12.8</v>
+        <v>11.1</v>
       </c>
       <c r="T6">
-        <v>0.012</v>
+        <v>0.017</v>
       </c>
       <c r="U6">
         <v>0.062</v>
       </c>
       <c r="V6">
-        <v>0.139</v>
+        <v>0.142</v>
       </c>
       <c r="W6">
-        <v>0.58</v>
+        <v>0.581</v>
       </c>
       <c r="X6">
-        <v>0.147</v>
+        <v>0.143</v>
       </c>
     </row>
     <row r="7" spans="1:24">
@@ -3664,34 +3664,34 @@
         <v>879</v>
       </c>
       <c r="O7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P7">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="Q7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="R7">
         <v>6</v>
       </c>
       <c r="S7">
-        <v>-0.3</v>
+        <v>1.4</v>
       </c>
       <c r="T7">
-        <v>0.035</v>
+        <v>0.033</v>
       </c>
       <c r="U7">
-        <v>0.14</v>
+        <v>0.137</v>
       </c>
       <c r="V7">
-        <v>0.154</v>
+        <v>0.156</v>
       </c>
       <c r="W7">
-        <v>0.659</v>
+        <v>0.6929999999999999</v>
       </c>
       <c r="X7">
-        <v>0.057</v>
+        <v>0.053</v>
       </c>
     </row>
     <row r="8" spans="1:24">
@@ -3738,16 +3738,16 @@
         <v>880</v>
       </c>
       <c r="O8">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P8">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="Q8">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="R8">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="S8">
         <v>14.1</v>
@@ -3756,13 +3756,13 @@
         <v>0.047</v>
       </c>
       <c r="U8">
-        <v>0.107</v>
+        <v>0.106</v>
       </c>
       <c r="V8">
-        <v>0.181</v>
+        <v>0.179</v>
       </c>
       <c r="W8">
-        <v>0.604</v>
+        <v>0.595</v>
       </c>
       <c r="X8">
         <v>0.096</v>
@@ -3812,7 +3812,7 @@
         <v>852</v>
       </c>
       <c r="O9">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P9">
         <v>15</v>
@@ -3824,19 +3824,19 @@
         <v>0</v>
       </c>
       <c r="S9">
-        <v>11.5</v>
+        <v>-2.2</v>
       </c>
       <c r="T9">
-        <v>0.038</v>
+        <v>0.031</v>
       </c>
       <c r="U9">
-        <v>0.098</v>
+        <v>0.08</v>
       </c>
       <c r="V9">
-        <v>0.206</v>
+        <v>0.254</v>
       </c>
       <c r="W9">
-        <v>0.375</v>
+        <v>0.259</v>
       </c>
       <c r="X9">
         <v>0</v>
@@ -4256,19 +4256,19 @@
         <v>852</v>
       </c>
       <c r="O15">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P15">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="Q15">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="R15">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="S15">
-        <v>10.6</v>
+        <v>12.4</v>
       </c>
       <c r="T15">
         <v>0.026</v>
@@ -4280,10 +4280,10 @@
         <v>0.135</v>
       </c>
       <c r="W15">
-        <v>0.463</v>
+        <v>0.489</v>
       </c>
       <c r="X15">
-        <v>0.163</v>
+        <v>0.162</v>
       </c>
     </row>
     <row r="16" spans="1:24">
@@ -4330,34 +4330,34 @@
         <v>852</v>
       </c>
       <c r="O16">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="P16">
         <v>3</v>
       </c>
       <c r="Q16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R16">
         <v>1</v>
       </c>
       <c r="S16">
-        <v>-2.5</v>
+        <v>-21.1</v>
       </c>
       <c r="T16">
-        <v>0</v>
+        <v>0.033</v>
       </c>
       <c r="U16">
-        <v>0.042</v>
+        <v>0.03</v>
       </c>
       <c r="V16">
-        <v>0.106</v>
+        <v>0.094</v>
       </c>
       <c r="W16">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="X16">
-        <v>0.067</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="17" spans="1:24">
@@ -4552,34 +4552,34 @@
         <v>875</v>
       </c>
       <c r="O19">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P19">
-        <v>398</v>
+        <v>414</v>
       </c>
       <c r="Q19">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="R19">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="S19">
-        <v>-16.3</v>
+        <v>-16.4</v>
       </c>
       <c r="T19">
-        <v>0.064</v>
+        <v>0.063</v>
       </c>
       <c r="U19">
-        <v>0.158</v>
+        <v>0.161</v>
       </c>
       <c r="V19">
-        <v>0.202</v>
+        <v>0.204</v>
       </c>
       <c r="W19">
-        <v>0.496</v>
+        <v>0.494</v>
       </c>
       <c r="X19">
-        <v>0.13</v>
+        <v>0.129</v>
       </c>
     </row>
     <row r="20" spans="1:24">
@@ -4700,34 +4700,34 @@
         <v>886</v>
       </c>
       <c r="O21">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P21">
-        <v>752</v>
+        <v>773</v>
       </c>
       <c r="Q21">
-        <v>406</v>
+        <v>416</v>
       </c>
       <c r="R21">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="S21">
-        <v>9.6</v>
+        <v>8.6</v>
       </c>
       <c r="T21">
-        <v>0.097</v>
+        <v>0.096</v>
       </c>
       <c r="U21">
-        <v>0.215</v>
+        <v>0.216</v>
       </c>
       <c r="V21">
-        <v>0.266</v>
+        <v>0.265</v>
       </c>
       <c r="W21">
-        <v>0.539</v>
+        <v>0.54</v>
       </c>
       <c r="X21">
-        <v>0.255</v>
+        <v>0.251</v>
       </c>
     </row>
     <row r="22" spans="1:24">
@@ -4774,22 +4774,22 @@
         <v>878</v>
       </c>
       <c r="O22">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P22">
-        <v>465</v>
+        <v>485</v>
       </c>
       <c r="Q22">
-        <v>287</v>
+        <v>297</v>
       </c>
       <c r="R22">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="S22">
-        <v>7.8</v>
+        <v>7</v>
       </c>
       <c r="T22">
-        <v>0.08</v>
+        <v>0.081</v>
       </c>
       <c r="U22">
         <v>0.162</v>
@@ -4798,10 +4798,10 @@
         <v>0.168</v>
       </c>
       <c r="W22">
-        <v>0.607</v>
+        <v>0.611</v>
       </c>
       <c r="X22">
-        <v>0.112</v>
+        <v>0.114</v>
       </c>
     </row>
     <row r="23" spans="1:24">
@@ -4848,19 +4848,19 @@
         <v>852</v>
       </c>
       <c r="O23">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P23">
-        <v>397</v>
+        <v>407</v>
       </c>
       <c r="Q23">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="R23">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="S23">
-        <v>2.2</v>
+        <v>2.6</v>
       </c>
       <c r="T23">
         <v>0.022</v>
@@ -4872,10 +4872,10 @@
         <v>0.154</v>
       </c>
       <c r="W23">
-        <v>0.618</v>
+        <v>0.621</v>
       </c>
       <c r="X23">
-        <v>0.066</v>
+        <v>0.067</v>
       </c>
     </row>
     <row r="24" spans="1:24">
@@ -5070,34 +5070,34 @@
         <v>889</v>
       </c>
       <c r="O26">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P26">
-        <v>277</v>
+        <v>289</v>
       </c>
       <c r="Q26">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="R26">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="S26">
-        <v>8.5</v>
+        <v>8.6</v>
       </c>
       <c r="T26">
-        <v>0.02</v>
+        <v>0.019</v>
       </c>
       <c r="U26">
         <v>0.096</v>
       </c>
       <c r="V26">
-        <v>0.178</v>
+        <v>0.179</v>
       </c>
       <c r="W26">
-        <v>0.551</v>
+        <v>0.545</v>
       </c>
       <c r="X26">
-        <v>0.243</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="27" spans="1:24">
@@ -5218,19 +5218,19 @@
         <v>890</v>
       </c>
       <c r="O28">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P28">
         <v>672</v>
       </c>
       <c r="Q28">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="R28">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="S28">
-        <v>-9</v>
+        <v>-10</v>
       </c>
       <c r="T28">
         <v>0.008999999999999999</v>
@@ -5239,13 +5239,13 @@
         <v>0.073</v>
       </c>
       <c r="V28">
-        <v>0.248</v>
+        <v>0.245</v>
       </c>
       <c r="W28">
-        <v>0.5570000000000001</v>
+        <v>0.549</v>
       </c>
       <c r="X28">
-        <v>0.252</v>
+        <v>0.253</v>
       </c>
     </row>
     <row r="29" spans="1:24">
@@ -5810,34 +5810,34 @@
         <v>885</v>
       </c>
       <c r="O36">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P36">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="Q36">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="R36">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="S36">
-        <v>0.1</v>
+        <v>-2.6</v>
       </c>
       <c r="T36">
-        <v>0.065</v>
+        <v>0.06900000000000001</v>
       </c>
       <c r="U36">
-        <v>0.178</v>
+        <v>0.18</v>
       </c>
       <c r="V36">
-        <v>0.181</v>
+        <v>0.183</v>
       </c>
       <c r="W36">
-        <v>0.547</v>
+        <v>0.536</v>
       </c>
       <c r="X36">
-        <v>0.14</v>
+        <v>0.146</v>
       </c>
     </row>
     <row r="37" spans="1:24">
@@ -5931,7 +5931,7 @@
         <v>549</v>
       </c>
       <c r="F38">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G38" t="s">
         <v>575</v>
@@ -6180,10 +6180,10 @@
         <v>895</v>
       </c>
       <c r="O41">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P41">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="Q41">
         <v>70</v>
@@ -6192,22 +6192,22 @@
         <v>29</v>
       </c>
       <c r="S41">
-        <v>-5.8</v>
+        <v>-5.2</v>
       </c>
       <c r="T41">
-        <v>0.028</v>
+        <v>0.027</v>
       </c>
       <c r="U41">
-        <v>0.094</v>
+        <v>0.091</v>
       </c>
       <c r="V41">
-        <v>0.11</v>
+        <v>0.108</v>
       </c>
       <c r="W41">
         <v>0.544</v>
       </c>
       <c r="X41">
-        <v>0.065</v>
+        <v>0.063</v>
       </c>
     </row>
     <row r="42" spans="1:24">
@@ -6402,34 +6402,34 @@
         <v>896</v>
       </c>
       <c r="O44">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P44">
-        <v>421</v>
+        <v>434</v>
       </c>
       <c r="Q44">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="R44">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="S44">
-        <v>-16.4</v>
+        <v>-16.5</v>
       </c>
       <c r="T44">
         <v>0.038</v>
       </c>
       <c r="U44">
-        <v>0.107</v>
+        <v>0.105</v>
       </c>
       <c r="V44">
         <v>0.173</v>
       </c>
       <c r="W44">
-        <v>0.519</v>
+        <v>0.52</v>
       </c>
       <c r="X44">
-        <v>0.151</v>
+        <v>0.148</v>
       </c>
     </row>
     <row r="45" spans="1:24">
@@ -6772,34 +6772,34 @@
         <v>901</v>
       </c>
       <c r="O49">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="P49">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="Q49">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="R49">
         <v>1</v>
       </c>
       <c r="S49">
-        <v>2.7</v>
+        <v>-1.2</v>
       </c>
       <c r="T49">
-        <v>0.089</v>
+        <v>0.102</v>
       </c>
       <c r="U49">
-        <v>0.148</v>
+        <v>0.143</v>
       </c>
       <c r="V49">
-        <v>0.203</v>
+        <v>0.202</v>
       </c>
       <c r="W49">
-        <v>0.647</v>
+        <v>0.659</v>
       </c>
       <c r="X49">
-        <v>0.034</v>
+        <v>0.031</v>
       </c>
     </row>
     <row r="50" spans="1:24">
@@ -6846,34 +6846,34 @@
         <v>895</v>
       </c>
       <c r="O50">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P50">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="Q50">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="R50">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="S50">
         <v>-6.9</v>
       </c>
       <c r="T50">
-        <v>0.024</v>
+        <v>0.023</v>
       </c>
       <c r="U50">
-        <v>0.083</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="V50">
-        <v>0.282</v>
+        <v>0.279</v>
       </c>
       <c r="W50">
-        <v>0.552</v>
+        <v>0.546</v>
       </c>
       <c r="X50">
-        <v>0.248</v>
+        <v>0.243</v>
       </c>
     </row>
     <row r="51" spans="1:24">
@@ -6994,34 +6994,34 @@
         <v>852</v>
       </c>
       <c r="O52">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P52">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="Q52">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="R52">
         <v>3</v>
       </c>
       <c r="S52">
-        <v>18.1</v>
+        <v>14.2</v>
       </c>
       <c r="T52">
-        <v>0.103</v>
+        <v>0.077</v>
       </c>
       <c r="U52">
-        <v>0.205</v>
+        <v>0.183</v>
       </c>
       <c r="V52">
-        <v>0.168</v>
+        <v>0.174</v>
       </c>
       <c r="W52">
-        <v>0.504</v>
+        <v>0.5679999999999999</v>
       </c>
       <c r="X52">
-        <v>0.097</v>
+        <v>0.073</v>
       </c>
     </row>
     <row r="53" spans="1:24">
@@ -8104,34 +8104,34 @@
         <v>874</v>
       </c>
       <c r="O67">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P67">
-        <v>883</v>
+        <v>903</v>
       </c>
       <c r="Q67">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="R67">
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="S67">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="T67">
-        <v>0.026</v>
+        <v>0.025</v>
       </c>
       <c r="U67">
-        <v>0.158</v>
+        <v>0.157</v>
       </c>
       <c r="V67">
         <v>0.311</v>
       </c>
       <c r="W67">
-        <v>0.556</v>
+        <v>0.553</v>
       </c>
       <c r="X67">
-        <v>0.418</v>
+        <v>0.416</v>
       </c>
     </row>
     <row r="68" spans="1:24">
@@ -8622,34 +8622,34 @@
         <v>913</v>
       </c>
       <c r="O74">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P74">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="Q74">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="R74">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="S74">
-        <v>6.4</v>
+        <v>6.5</v>
       </c>
       <c r="T74">
-        <v>0.041</v>
+        <v>0.039</v>
       </c>
       <c r="U74">
-        <v>0.14</v>
+        <v>0.138</v>
       </c>
       <c r="V74">
-        <v>0.254</v>
+        <v>0.25</v>
       </c>
       <c r="W74">
-        <v>0.547</v>
+        <v>0.545</v>
       </c>
       <c r="X74">
-        <v>0.055</v>
+        <v>0.063</v>
       </c>
     </row>
     <row r="75" spans="1:24">
@@ -8844,34 +8844,34 @@
         <v>913</v>
       </c>
       <c r="O77">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P77">
-        <v>367</v>
+        <v>376</v>
       </c>
       <c r="Q77">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="R77">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="S77">
-        <v>15.2</v>
+        <v>13.2</v>
       </c>
       <c r="T77">
-        <v>0.025</v>
+        <v>0.024</v>
       </c>
       <c r="U77">
-        <v>0.08799999999999999</v>
+        <v>0.089</v>
       </c>
       <c r="V77">
-        <v>0.18</v>
+        <v>0.181</v>
       </c>
       <c r="W77">
         <v>0.611</v>
       </c>
       <c r="X77">
-        <v>0.201</v>
+        <v>0.202</v>
       </c>
     </row>
     <row r="78" spans="1:24">
@@ -8918,34 +8918,34 @@
         <v>879</v>
       </c>
       <c r="O78">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P78">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="Q78">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="R78">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="S78">
-        <v>-18.4</v>
+        <v>-18.7</v>
       </c>
       <c r="T78">
         <v>0.01</v>
       </c>
       <c r="U78">
-        <v>0.123</v>
+        <v>0.124</v>
       </c>
       <c r="V78">
-        <v>0.139</v>
+        <v>0.138</v>
       </c>
       <c r="W78">
-        <v>0.512</v>
+        <v>0.509</v>
       </c>
       <c r="X78">
-        <v>0.19</v>
+        <v>0.189</v>
       </c>
     </row>
     <row r="79" spans="1:24">
@@ -8992,34 +8992,34 @@
         <v>906</v>
       </c>
       <c r="O79">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P79">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="Q79">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="R79">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="S79">
-        <v>13.1</v>
+        <v>13.4</v>
       </c>
       <c r="T79">
-        <v>0.037</v>
+        <v>0.036</v>
       </c>
       <c r="U79">
-        <v>0.073</v>
+        <v>0.077</v>
       </c>
       <c r="V79">
         <v>0.114</v>
       </c>
       <c r="W79">
-        <v>0.537</v>
+        <v>0.536</v>
       </c>
       <c r="X79">
-        <v>0.112</v>
+        <v>0.111</v>
       </c>
     </row>
     <row r="80" spans="1:24">
@@ -10398,34 +10398,34 @@
         <v>917</v>
       </c>
       <c r="O98">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P98">
-        <v>375</v>
+        <v>389</v>
       </c>
       <c r="Q98">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="R98">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="S98">
-        <v>-11.7</v>
+        <v>-10.5</v>
       </c>
       <c r="T98">
-        <v>0.016</v>
+        <v>0.017</v>
       </c>
       <c r="U98">
         <v>0.08699999999999999</v>
       </c>
       <c r="V98">
-        <v>0.167</v>
+        <v>0.168</v>
       </c>
       <c r="W98">
-        <v>0.576</v>
+        <v>0.573</v>
       </c>
       <c r="X98">
-        <v>0.09</v>
+        <v>0.094</v>
       </c>
     </row>
     <row r="99" spans="1:24">
@@ -10546,34 +10546,34 @@
         <v>852</v>
       </c>
       <c r="O100">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P100">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="Q100">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R100">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="S100">
-        <v>-3.4</v>
+        <v>-0.5</v>
       </c>
       <c r="T100">
-        <v>0.013</v>
+        <v>0.019</v>
       </c>
       <c r="U100">
-        <v>0.075</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="V100">
-        <v>0.123</v>
+        <v>0.127</v>
       </c>
       <c r="W100">
-        <v>0.633</v>
+        <v>0.674</v>
       </c>
       <c r="X100">
-        <v>0.18</v>
+        <v>0.196</v>
       </c>
     </row>
     <row r="101" spans="1:24">
@@ -11064,34 +11064,34 @@
         <v>911</v>
       </c>
       <c r="O107">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P107">
-        <v>259</v>
+        <v>282</v>
       </c>
       <c r="Q107">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="R107">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="S107">
-        <v>3</v>
+        <v>1.6</v>
       </c>
       <c r="T107">
-        <v>0.023</v>
+        <v>0.021</v>
       </c>
       <c r="U107">
-        <v>0.1</v>
+        <v>0.102</v>
       </c>
       <c r="V107">
-        <v>0.257</v>
+        <v>0.261</v>
       </c>
       <c r="W107">
-        <v>0.515</v>
+        <v>0.52</v>
       </c>
       <c r="X107">
-        <v>0.227</v>
+        <v>0.222</v>
       </c>
     </row>
     <row r="108" spans="1:24">
@@ -11804,34 +11804,34 @@
         <v>885</v>
       </c>
       <c r="O117">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P117">
-        <v>799</v>
+        <v>819</v>
       </c>
       <c r="Q117">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="R117">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="S117">
-        <v>11.8</v>
+        <v>10.8</v>
       </c>
       <c r="T117">
-        <v>0.015</v>
+        <v>0.016</v>
       </c>
       <c r="U117">
         <v>0.064</v>
       </c>
       <c r="V117">
-        <v>0.263</v>
+        <v>0.262</v>
       </c>
       <c r="W117">
-        <v>0.633</v>
+        <v>0.636</v>
       </c>
       <c r="X117">
-        <v>0.302</v>
+        <v>0.307</v>
       </c>
     </row>
     <row r="118" spans="1:24">
@@ -12174,16 +12174,16 @@
         <v>885</v>
       </c>
       <c r="O122">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P122">
-        <v>979</v>
+        <v>998</v>
       </c>
       <c r="Q122">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="R122">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="S122">
         <v>1.4</v>
@@ -12192,16 +12192,16 @@
         <v>0.029</v>
       </c>
       <c r="U122">
-        <v>0.108</v>
+        <v>0.106</v>
       </c>
       <c r="V122">
-        <v>0.293</v>
+        <v>0.291</v>
       </c>
       <c r="W122">
-        <v>0.579</v>
+        <v>0.577</v>
       </c>
       <c r="X122">
-        <v>0.261</v>
+        <v>0.259</v>
       </c>
     </row>
     <row r="123" spans="1:24">
@@ -12470,19 +12470,19 @@
         <v>887</v>
       </c>
       <c r="O126">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P126">
-        <v>740</v>
+        <v>773</v>
       </c>
       <c r="Q126">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="R126">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="S126">
-        <v>3.5</v>
+        <v>3.8</v>
       </c>
       <c r="T126">
         <v>0.014</v>
@@ -12491,10 +12491,10 @@
         <v>0.09</v>
       </c>
       <c r="V126">
-        <v>0.238</v>
+        <v>0.239</v>
       </c>
       <c r="W126">
-        <v>0.5620000000000001</v>
+        <v>0.5649999999999999</v>
       </c>
       <c r="X126">
         <v>0.159</v>
@@ -12544,19 +12544,19 @@
         <v>852</v>
       </c>
       <c r="O127">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P127">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="Q127">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="R127">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="S127">
-        <v>12.9</v>
+        <v>11.6</v>
       </c>
       <c r="T127">
         <v>0.04</v>
@@ -12568,10 +12568,10 @@
         <v>0.101</v>
       </c>
       <c r="W127">
-        <v>0.5639999999999999</v>
+        <v>0.569</v>
       </c>
       <c r="X127">
-        <v>0.075</v>
+        <v>0.073</v>
       </c>
     </row>
     <row r="128" spans="1:24">
@@ -12618,34 +12618,34 @@
         <v>874</v>
       </c>
       <c r="O128">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="P128">
-        <v>391</v>
+        <v>405</v>
       </c>
       <c r="Q128">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="R128">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="S128">
-        <v>-11.5</v>
+        <v>-12.6</v>
       </c>
       <c r="T128">
-        <v>0.089</v>
+        <v>0.09</v>
       </c>
       <c r="U128">
-        <v>0.246</v>
+        <v>0.247</v>
       </c>
       <c r="V128">
-        <v>0.189</v>
+        <v>0.191</v>
       </c>
       <c r="W128">
-        <v>0.579</v>
+        <v>0.578</v>
       </c>
       <c r="X128">
-        <v>0.076</v>
+        <v>0.077</v>
       </c>
     </row>
     <row r="129" spans="1:24">
@@ -13062,34 +13062,34 @@
         <v>852</v>
       </c>
       <c r="O134">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P134">
-        <v>359</v>
+        <v>372</v>
       </c>
       <c r="Q134">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="R134">
         <v>32</v>
       </c>
       <c r="S134">
-        <v>2.7</v>
+        <v>3.3</v>
       </c>
       <c r="T134">
-        <v>0.046</v>
+        <v>0.047</v>
       </c>
       <c r="U134">
         <v>0.089</v>
       </c>
       <c r="V134">
-        <v>0.162</v>
+        <v>0.163</v>
       </c>
       <c r="W134">
-        <v>0.592</v>
+        <v>0.596</v>
       </c>
       <c r="X134">
-        <v>0.053</v>
+        <v>0.052</v>
       </c>
     </row>
     <row r="135" spans="1:24">
@@ -13284,34 +13284,34 @@
         <v>915</v>
       </c>
       <c r="O137">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P137">
-        <v>856</v>
+        <v>893</v>
       </c>
       <c r="Q137">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="R137">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="S137">
-        <v>-1.2</v>
+        <v>-0.7</v>
       </c>
       <c r="T137">
-        <v>0.031</v>
+        <v>0.03</v>
       </c>
       <c r="U137">
-        <v>0.075</v>
+        <v>0.074</v>
       </c>
       <c r="V137">
-        <v>0.281</v>
+        <v>0.283</v>
       </c>
       <c r="W137">
-        <v>0.583</v>
+        <v>0.584</v>
       </c>
       <c r="X137">
-        <v>0.294</v>
+        <v>0.291</v>
       </c>
     </row>
     <row r="138" spans="1:24">
@@ -13358,34 +13358,34 @@
         <v>915</v>
       </c>
       <c r="O138">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P138">
         <v>34</v>
       </c>
       <c r="Q138">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R138">
         <v>11</v>
       </c>
       <c r="S138">
-        <v>1.6</v>
+        <v>-2</v>
       </c>
       <c r="T138">
-        <v>0.04</v>
+        <v>0.037</v>
       </c>
       <c r="U138">
-        <v>0.221</v>
+        <v>0.214</v>
       </c>
       <c r="V138">
-        <v>0.191</v>
+        <v>0.18</v>
       </c>
       <c r="W138">
-        <v>0.455</v>
+        <v>0.443</v>
       </c>
       <c r="X138">
-        <v>0.183</v>
+        <v>0.162</v>
       </c>
     </row>
     <row r="139" spans="1:24">
@@ -13506,19 +13506,19 @@
         <v>923</v>
       </c>
       <c r="O140">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P140">
-        <v>469</v>
+        <v>481</v>
       </c>
       <c r="Q140">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="R140">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="S140">
-        <v>8.1</v>
+        <v>7.8</v>
       </c>
       <c r="T140">
         <v>0.036</v>
@@ -13527,13 +13527,13 @@
         <v>0.079</v>
       </c>
       <c r="V140">
-        <v>0.171</v>
+        <v>0.172</v>
       </c>
       <c r="W140">
-        <v>0.532</v>
+        <v>0.528</v>
       </c>
       <c r="X140">
-        <v>0.07099999999999999</v>
+        <v>0.073</v>
       </c>
     </row>
     <row r="141" spans="1:24">
@@ -13654,34 +13654,34 @@
         <v>914</v>
       </c>
       <c r="O142">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P142">
-        <v>761</v>
+        <v>781</v>
       </c>
       <c r="Q142">
-        <v>522</v>
+        <v>536</v>
       </c>
       <c r="R142">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="S142">
-        <v>4.8</v>
+        <v>5.3</v>
       </c>
       <c r="T142">
-        <v>0.105</v>
+        <v>0.106</v>
       </c>
       <c r="U142">
-        <v>0.283</v>
+        <v>0.282</v>
       </c>
       <c r="V142">
-        <v>0.213</v>
+        <v>0.212</v>
       </c>
       <c r="W142">
         <v>0.67</v>
       </c>
       <c r="X142">
-        <v>0.257</v>
+        <v>0.256</v>
       </c>
     </row>
     <row r="143" spans="1:24">
@@ -13876,31 +13876,31 @@
         <v>915</v>
       </c>
       <c r="O145">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P145">
-        <v>856</v>
+        <v>864</v>
       </c>
       <c r="Q145">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="R145">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="S145">
-        <v>11.5</v>
+        <v>10.2</v>
       </c>
       <c r="T145">
-        <v>0.019</v>
+        <v>0.018</v>
       </c>
       <c r="U145">
         <v>0.118</v>
       </c>
       <c r="V145">
-        <v>0.289</v>
+        <v>0.29</v>
       </c>
       <c r="W145">
-        <v>0.587</v>
+        <v>0.579</v>
       </c>
       <c r="X145">
         <v>0.218</v>
@@ -14542,10 +14542,10 @@
         <v>852</v>
       </c>
       <c r="O154">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P154">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="Q154">
         <v>19</v>
@@ -14554,22 +14554,22 @@
         <v>5</v>
       </c>
       <c r="S154">
-        <v>-18.2</v>
+        <v>-17</v>
       </c>
       <c r="T154">
         <v>0.058</v>
       </c>
       <c r="U154">
-        <v>0.115</v>
+        <v>0.111</v>
       </c>
       <c r="V154">
-        <v>0.16</v>
+        <v>0.168</v>
       </c>
       <c r="W154">
-        <v>0.516</v>
+        <v>0.527</v>
       </c>
       <c r="X154">
-        <v>0.066</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="155" spans="1:24">
@@ -15134,31 +15134,31 @@
         <v>883</v>
       </c>
       <c r="O162">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P162">
-        <v>702</v>
+        <v>707</v>
       </c>
       <c r="Q162">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="R162">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="S162">
-        <v>14.8</v>
+        <v>13.5</v>
       </c>
       <c r="T162">
         <v>0.07000000000000001</v>
       </c>
       <c r="U162">
-        <v>0.212</v>
+        <v>0.211</v>
       </c>
       <c r="V162">
-        <v>0.228</v>
+        <v>0.227</v>
       </c>
       <c r="W162">
-        <v>0.658</v>
+        <v>0.653</v>
       </c>
       <c r="X162">
         <v>0.137</v>
@@ -15800,34 +15800,34 @@
         <v>924</v>
       </c>
       <c r="O171">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P171">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="Q171">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="R171">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="S171">
-        <v>10.7</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="T171">
-        <v>0.034</v>
+        <v>0.033</v>
       </c>
       <c r="U171">
-        <v>0.134</v>
+        <v>0.135</v>
       </c>
       <c r="V171">
-        <v>0.169</v>
+        <v>0.17</v>
       </c>
       <c r="W171">
-        <v>0.605</v>
+        <v>0.598</v>
       </c>
       <c r="X171">
-        <v>0.097</v>
+        <v>0.098</v>
       </c>
     </row>
     <row r="172" spans="1:24">
@@ -16170,34 +16170,34 @@
         <v>904</v>
       </c>
       <c r="O176">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P176">
-        <v>327</v>
+        <v>348</v>
       </c>
       <c r="Q176">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="R176">
         <v>55</v>
       </c>
       <c r="S176">
-        <v>-1.1</v>
+        <v>-0.8</v>
       </c>
       <c r="T176">
-        <v>0.025</v>
+        <v>0.024</v>
       </c>
       <c r="U176">
-        <v>0.102</v>
+        <v>0.105</v>
       </c>
       <c r="V176">
-        <v>0.171</v>
+        <v>0.173</v>
       </c>
       <c r="W176">
-        <v>0.632</v>
+        <v>0.643</v>
       </c>
       <c r="X176">
-        <v>0.109</v>
+        <v>0.105</v>
       </c>
     </row>
     <row r="177" spans="1:24">
@@ -16904,34 +16904,34 @@
         <v>885</v>
       </c>
       <c r="O186">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P186">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="Q186">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="R186">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="S186">
-        <v>11.8</v>
+        <v>12.5</v>
       </c>
       <c r="T186">
-        <v>0.044</v>
+        <v>0.043</v>
       </c>
       <c r="U186">
-        <v>0.061</v>
+        <v>0.063</v>
       </c>
       <c r="V186">
-        <v>0.114</v>
+        <v>0.118</v>
       </c>
       <c r="W186">
-        <v>0.583</v>
+        <v>0.5669999999999999</v>
       </c>
       <c r="X186">
-        <v>0.099</v>
+        <v>0.096</v>
       </c>
     </row>
     <row r="187" spans="1:24">
@@ -17274,34 +17274,34 @@
         <v>927</v>
       </c>
       <c r="O191">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P191">
-        <v>325</v>
+        <v>337</v>
       </c>
       <c r="Q191">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="R191">
         <v>53</v>
       </c>
       <c r="S191">
-        <v>15.5</v>
+        <v>16</v>
       </c>
       <c r="T191">
         <v>0.021</v>
       </c>
       <c r="U191">
-        <v>0.094</v>
+        <v>0.095</v>
       </c>
       <c r="V191">
-        <v>0.167</v>
+        <v>0.166</v>
       </c>
       <c r="W191">
-        <v>0.5590000000000001</v>
+        <v>0.5659999999999999</v>
       </c>
       <c r="X191">
-        <v>0.089</v>
+        <v>0.08599999999999999</v>
       </c>
     </row>
     <row r="192" spans="1:24">
@@ -17348,34 +17348,34 @@
         <v>886</v>
       </c>
       <c r="O192">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P192">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="Q192">
-        <v>208</v>
+        <v>221</v>
       </c>
       <c r="R192">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="S192">
-        <v>-3.5</v>
+        <v>-3</v>
       </c>
       <c r="T192">
-        <v>0.096</v>
+        <v>0.098</v>
       </c>
       <c r="U192">
-        <v>0.165</v>
+        <v>0.17</v>
       </c>
       <c r="V192">
         <v>0.112</v>
       </c>
       <c r="W192">
-        <v>0.587</v>
+        <v>0.58</v>
       </c>
       <c r="X192">
-        <v>0.118</v>
+        <v>0.123</v>
       </c>
     </row>
     <row r="193" spans="1:24">
@@ -17496,31 +17496,31 @@
         <v>910</v>
       </c>
       <c r="O194">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P194">
-        <v>585</v>
+        <v>595</v>
       </c>
       <c r="Q194">
-        <v>492</v>
+        <v>500</v>
       </c>
       <c r="R194">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="S194">
-        <v>5.3</v>
+        <v>6.3</v>
       </c>
       <c r="T194">
-        <v>0.122</v>
+        <v>0.121</v>
       </c>
       <c r="U194">
-        <v>0.274</v>
+        <v>0.273</v>
       </c>
       <c r="V194">
-        <v>0.185</v>
+        <v>0.184</v>
       </c>
       <c r="W194">
-        <v>0.62</v>
+        <v>0.618</v>
       </c>
       <c r="X194">
         <v>0.123</v>
@@ -17940,34 +17940,34 @@
         <v>928</v>
       </c>
       <c r="O200">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P200">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="Q200">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="R200">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="S200">
-        <v>-7</v>
+        <v>-6.3</v>
       </c>
       <c r="T200">
         <v>0.07000000000000001</v>
       </c>
       <c r="U200">
-        <v>0.202</v>
+        <v>0.204</v>
       </c>
       <c r="V200">
-        <v>0.146</v>
+        <v>0.142</v>
       </c>
       <c r="W200">
-        <v>0.512</v>
+        <v>0.5</v>
       </c>
       <c r="X200">
-        <v>0.07099999999999999</v>
+        <v>0.07199999999999999</v>
       </c>
     </row>
     <row r="201" spans="1:24">
@@ -18976,34 +18976,34 @@
         <v>915</v>
       </c>
       <c r="O214">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P214">
-        <v>352</v>
+        <v>369</v>
       </c>
       <c r="Q214">
-        <v>347</v>
+        <v>364</v>
       </c>
       <c r="R214">
         <v>87</v>
       </c>
       <c r="S214">
-        <v>-2.8</v>
+        <v>-3.5</v>
       </c>
       <c r="T214">
-        <v>0.13</v>
+        <v>0.132</v>
       </c>
       <c r="U214">
-        <v>0.247</v>
+        <v>0.252</v>
       </c>
       <c r="V214">
         <v>0.149</v>
       </c>
       <c r="W214">
-        <v>0.6909999999999999</v>
+        <v>0.702</v>
       </c>
       <c r="X214">
-        <v>0.133</v>
+        <v>0.131</v>
       </c>
     </row>
     <row r="215" spans="1:24">
@@ -19050,34 +19050,34 @@
         <v>875</v>
       </c>
       <c r="O215">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P215">
-        <v>832</v>
+        <v>860</v>
       </c>
       <c r="Q215">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="R215">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="S215">
-        <v>4.7</v>
+        <v>4.5</v>
       </c>
       <c r="T215">
         <v>0.015</v>
       </c>
       <c r="U215">
-        <v>0.112</v>
+        <v>0.113</v>
       </c>
       <c r="V215">
-        <v>0.261</v>
+        <v>0.262</v>
       </c>
       <c r="W215">
-        <v>0.5620000000000001</v>
+        <v>0.5639999999999999</v>
       </c>
       <c r="X215">
-        <v>0.125</v>
+        <v>0.126</v>
       </c>
     </row>
     <row r="216" spans="1:24">
@@ -19494,19 +19494,19 @@
         <v>884</v>
       </c>
       <c r="O221">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P221">
-        <v>805</v>
+        <v>824</v>
       </c>
       <c r="Q221">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="R221">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="S221">
-        <v>11.4</v>
+        <v>12.1</v>
       </c>
       <c r="T221">
         <v>0.025</v>
@@ -19515,13 +19515,13 @@
         <v>0.14</v>
       </c>
       <c r="V221">
-        <v>0.27</v>
+        <v>0.268</v>
       </c>
       <c r="W221">
-        <v>0.5610000000000001</v>
+        <v>0.5629999999999999</v>
       </c>
       <c r="X221">
-        <v>0.245</v>
+        <v>0.242</v>
       </c>
     </row>
     <row r="222" spans="1:24">
@@ -19864,34 +19864,34 @@
         <v>883</v>
       </c>
       <c r="O226">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P226">
-        <v>796</v>
+        <v>815</v>
       </c>
       <c r="Q226">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="R226">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="S226">
-        <v>4.1</v>
+        <v>4.5</v>
       </c>
       <c r="T226">
-        <v>0.017</v>
+        <v>0.018</v>
       </c>
       <c r="U226">
-        <v>0.157</v>
+        <v>0.153</v>
       </c>
       <c r="V226">
         <v>0.295</v>
       </c>
       <c r="W226">
-        <v>0.572</v>
+        <v>0.571</v>
       </c>
       <c r="X226">
-        <v>0.373</v>
+        <v>0.371</v>
       </c>
     </row>
     <row r="227" spans="1:24">
@@ -20160,19 +20160,19 @@
         <v>918</v>
       </c>
       <c r="O230">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P230">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="Q230">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="R230">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="S230">
-        <v>-8.6</v>
+        <v>-7.6</v>
       </c>
       <c r="T230">
         <v>0.023</v>
@@ -20184,10 +20184,10 @@
         <v>0.161</v>
       </c>
       <c r="W230">
-        <v>0.588</v>
+        <v>0.591</v>
       </c>
       <c r="X230">
-        <v>0.116</v>
+        <v>0.115</v>
       </c>
     </row>
     <row r="231" spans="1:24">
@@ -20234,34 +20234,34 @@
         <v>909</v>
       </c>
       <c r="O231">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="P231">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="Q231">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="R231">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="S231">
-        <v>-6</v>
+        <v>-3.7</v>
       </c>
       <c r="T231">
-        <v>0.034</v>
+        <v>0.033</v>
       </c>
       <c r="U231">
-        <v>0.07099999999999999</v>
+        <v>0.074</v>
       </c>
       <c r="V231">
-        <v>0.248</v>
+        <v>0.244</v>
       </c>
       <c r="W231">
-        <v>0.57</v>
+        <v>0.571</v>
       </c>
       <c r="X231">
-        <v>0.371</v>
+        <v>0.358</v>
       </c>
     </row>
     <row r="232" spans="1:24">
@@ -20530,31 +20530,31 @@
         <v>898</v>
       </c>
       <c r="O235">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P235">
-        <v>551</v>
+        <v>564</v>
       </c>
       <c r="Q235">
-        <v>397</v>
+        <v>404</v>
       </c>
       <c r="R235">
         <v>77</v>
       </c>
       <c r="S235">
-        <v>9.9</v>
+        <v>9</v>
       </c>
       <c r="T235">
-        <v>0.091</v>
+        <v>0.092</v>
       </c>
       <c r="U235">
         <v>0.253</v>
       </c>
       <c r="V235">
-        <v>0.154</v>
+        <v>0.155</v>
       </c>
       <c r="W235">
-        <v>0.726</v>
+        <v>0.73</v>
       </c>
       <c r="X235">
         <v>0.08699999999999999</v>
@@ -21193,34 +21193,34 @@
         <v>908</v>
       </c>
       <c r="O244">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="P244">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="Q244">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="R244">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S244">
-        <v>11.6</v>
+        <v>12.3</v>
       </c>
       <c r="T244">
-        <v>0.066</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="U244">
-        <v>0.209</v>
+        <v>0.205</v>
       </c>
       <c r="V244">
-        <v>0.147</v>
+        <v>0.149</v>
       </c>
       <c r="W244">
-        <v>0.5629999999999999</v>
+        <v>0.546</v>
       </c>
       <c r="X244">
-        <v>0.217</v>
+        <v>0.201</v>
       </c>
     </row>
     <row r="245" spans="1:24">
@@ -21267,34 +21267,34 @@
         <v>913</v>
       </c>
       <c r="O245">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P245">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="Q245">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="R245">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="S245">
-        <v>-9.199999999999999</v>
+        <v>-3.8</v>
       </c>
       <c r="T245">
-        <v>0.08</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="U245">
-        <v>0.126</v>
+        <v>0.133</v>
       </c>
       <c r="V245">
-        <v>0.138</v>
+        <v>0.144</v>
       </c>
       <c r="W245">
-        <v>0.472</v>
+        <v>0.465</v>
       </c>
       <c r="X245">
-        <v>0.138</v>
+        <v>0.133</v>
       </c>
     </row>
     <row r="246" spans="1:24">
@@ -21563,34 +21563,34 @@
         <v>885</v>
       </c>
       <c r="O249">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="P249">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="Q249">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="R249">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S249">
-        <v>-11.3</v>
+        <v>-10.8</v>
       </c>
       <c r="T249">
-        <v>0.008</v>
+        <v>0.013</v>
       </c>
       <c r="U249">
-        <v>0.109</v>
+        <v>0.103</v>
       </c>
       <c r="V249">
-        <v>0.135</v>
+        <v>0.131</v>
       </c>
       <c r="W249">
-        <v>0.652</v>
+        <v>0.671</v>
       </c>
       <c r="X249">
-        <v>0.013</v>
+        <v>0.031</v>
       </c>
     </row>
     <row r="250" spans="1:24">
@@ -22747,34 +22747,34 @@
         <v>885</v>
       </c>
       <c r="O265">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P265">
-        <v>442</v>
+        <v>453</v>
       </c>
       <c r="Q265">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="R265">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="S265">
-        <v>-15.1</v>
+        <v>-14.4</v>
       </c>
       <c r="T265">
-        <v>0.12</v>
+        <v>0.121</v>
       </c>
       <c r="U265">
-        <v>0.276</v>
+        <v>0.279</v>
       </c>
       <c r="V265">
         <v>0.236</v>
       </c>
       <c r="W265">
-        <v>0.61</v>
+        <v>0.612</v>
       </c>
       <c r="X265">
-        <v>0.188</v>
+        <v>0.185</v>
       </c>
     </row>
     <row r="266" spans="1:24">
@@ -23265,7 +23265,7 @@
         <v>925</v>
       </c>
       <c r="O272">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P272">
         <v>134</v>
@@ -23277,22 +23277,22 @@
         <v>30</v>
       </c>
       <c r="S272">
-        <v>-2.1</v>
+        <v>-2.2</v>
       </c>
       <c r="T272">
-        <v>0.06</v>
+        <v>0.059</v>
       </c>
       <c r="U272">
-        <v>0.08500000000000001</v>
+        <v>0.08400000000000001</v>
       </c>
       <c r="V272">
-        <v>0.188</v>
+        <v>0.185</v>
       </c>
       <c r="W272">
-        <v>0.502</v>
+        <v>0.498</v>
       </c>
       <c r="X272">
-        <v>0.136</v>
+        <v>0.132</v>
       </c>
     </row>
     <row r="273" spans="1:24">
@@ -23339,34 +23339,34 @@
         <v>905</v>
       </c>
       <c r="O273">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P273">
-        <v>666</v>
+        <v>684</v>
       </c>
       <c r="Q273">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="R273">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="S273">
-        <v>-13.2</v>
+        <v>-13.9</v>
       </c>
       <c r="T273">
         <v>0.012</v>
       </c>
       <c r="U273">
-        <v>0.07199999999999999</v>
+        <v>0.074</v>
       </c>
       <c r="V273">
-        <v>0.283</v>
+        <v>0.284</v>
       </c>
       <c r="W273">
-        <v>0.593</v>
+        <v>0.591</v>
       </c>
       <c r="X273">
-        <v>0.255</v>
+        <v>0.256</v>
       </c>
     </row>
     <row r="274" spans="1:24">
@@ -24449,13 +24449,13 @@
         <v>852</v>
       </c>
       <c r="O288">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P288">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="Q288">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="R288">
         <v>23</v>
@@ -24464,19 +24464,19 @@
         <v>-9.300000000000001</v>
       </c>
       <c r="T288">
-        <v>0.075</v>
+        <v>0.077</v>
       </c>
       <c r="U288">
+        <v>0.14</v>
+      </c>
+      <c r="V288">
         <v>0.142</v>
       </c>
-      <c r="V288">
-        <v>0.14</v>
-      </c>
       <c r="W288">
-        <v>0.638</v>
+        <v>0.646</v>
       </c>
       <c r="X288">
-        <v>0.066</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="289" spans="1:24">
@@ -24597,7 +24597,7 @@
         <v>852</v>
       </c>
       <c r="O290">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P290">
         <v>0</v>
@@ -24609,22 +24609,22 @@
         <v>1</v>
       </c>
       <c r="S290">
-        <v>-47.6</v>
+        <v>-28.6</v>
       </c>
       <c r="T290">
-        <v>0.143</v>
+        <v>0.125</v>
       </c>
       <c r="U290">
-        <v>0.143</v>
+        <v>0.083</v>
       </c>
       <c r="V290">
-        <v>0.037</v>
+        <v>0.029</v>
       </c>
       <c r="W290">
         <v>0</v>
       </c>
       <c r="X290">
-        <v>0.25</v>
+        <v>0.143</v>
       </c>
     </row>
     <row r="291" spans="1:24">
@@ -24893,7 +24893,7 @@
         <v>902</v>
       </c>
       <c r="O294">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P294">
         <v>57</v>
@@ -24905,22 +24905,22 @@
         <v>10</v>
       </c>
       <c r="S294">
-        <v>-2.5</v>
+        <v>-3</v>
       </c>
       <c r="T294">
-        <v>0.07000000000000001</v>
+        <v>0.06900000000000001</v>
       </c>
       <c r="U294">
         <v>0.138</v>
       </c>
       <c r="V294">
-        <v>0.104</v>
+        <v>0.103</v>
       </c>
       <c r="W294">
         <v>0.726</v>
       </c>
       <c r="X294">
-        <v>0.081</v>
+        <v>0.079</v>
       </c>
     </row>
     <row r="295" spans="1:24">
@@ -25263,34 +25263,34 @@
         <v>878</v>
       </c>
       <c r="O299">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P299">
-        <v>441</v>
+        <v>459</v>
       </c>
       <c r="Q299">
-        <v>267</v>
+        <v>278</v>
       </c>
       <c r="R299">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="S299">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
       <c r="T299">
-        <v>0.058</v>
+        <v>0.059</v>
       </c>
       <c r="U299">
-        <v>0.137</v>
+        <v>0.139</v>
       </c>
       <c r="V299">
-        <v>0.146</v>
+        <v>0.144</v>
       </c>
       <c r="W299">
-        <v>0.521</v>
+        <v>0.529</v>
       </c>
       <c r="X299">
-        <v>0.051</v>
+        <v>0.052</v>
       </c>
     </row>
     <row r="300" spans="1:24">
@@ -25633,34 +25633,34 @@
         <v>852</v>
       </c>
       <c r="O304">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="P304">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="Q304">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="R304">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="S304">
-        <v>16.7</v>
+        <v>16.1</v>
       </c>
       <c r="T304">
-        <v>0.057</v>
+        <v>0.055</v>
       </c>
       <c r="U304">
-        <v>0.156</v>
+        <v>0.155</v>
       </c>
       <c r="V304">
-        <v>0.162</v>
+        <v>0.161</v>
       </c>
       <c r="W304">
-        <v>0.637</v>
+        <v>0.63</v>
       </c>
       <c r="X304">
-        <v>0.094</v>
+        <v>0.097</v>
       </c>
     </row>
     <row r="305" spans="1:24">
@@ -25781,13 +25781,13 @@
         <v>852</v>
       </c>
       <c r="O306">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P306">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="Q306">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="R306">
         <v>45</v>
@@ -25796,7 +25796,7 @@
         <v>9.300000000000001</v>
       </c>
       <c r="T306">
-        <v>0.038</v>
+        <v>0.037</v>
       </c>
       <c r="U306">
         <v>0.074</v>
@@ -25805,10 +25805,10 @@
         <v>0.126</v>
       </c>
       <c r="W306">
-        <v>0.648</v>
+        <v>0.653</v>
       </c>
       <c r="X306">
-        <v>0.07000000000000001</v>
+        <v>0.06900000000000001</v>
       </c>
     </row>
     <row r="307" spans="1:24">
@@ -26077,34 +26077,34 @@
         <v>875</v>
       </c>
       <c r="O310">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="P310">
-        <v>790</v>
+        <v>813</v>
       </c>
       <c r="Q310">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="R310">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="S310">
-        <v>-1.1</v>
+        <v>-0.2</v>
       </c>
       <c r="T310">
         <v>0.014</v>
       </c>
       <c r="U310">
-        <v>0.153</v>
+        <v>0.152</v>
       </c>
       <c r="V310">
-        <v>0.302</v>
+        <v>0.3</v>
       </c>
       <c r="W310">
-        <v>0.63</v>
+        <v>0.629</v>
       </c>
       <c r="X310">
-        <v>0.2</v>
+        <v>0.197</v>
       </c>
     </row>
     <row r="311" spans="1:24">
@@ -26151,19 +26151,19 @@
         <v>902</v>
       </c>
       <c r="O311">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P311">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="Q311">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="R311">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="S311">
-        <v>-2.4</v>
+        <v>-2.5</v>
       </c>
       <c r="T311">
         <v>0.021</v>
@@ -26172,10 +26172,10 @@
         <v>0.112</v>
       </c>
       <c r="V311">
-        <v>0.165</v>
+        <v>0.166</v>
       </c>
       <c r="W311">
-        <v>0.535</v>
+        <v>0.537</v>
       </c>
       <c r="X311">
         <v>0.113</v>
@@ -26299,19 +26299,19 @@
         <v>894</v>
       </c>
       <c r="O313">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P313">
-        <v>327</v>
+        <v>335</v>
       </c>
       <c r="Q313">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="R313">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="S313">
-        <v>-2.2</v>
+        <v>-0.8</v>
       </c>
       <c r="T313">
         <v>0.032</v>
@@ -26323,10 +26323,10 @@
         <v>0.262</v>
       </c>
       <c r="W313">
-        <v>0.473</v>
+        <v>0.477</v>
       </c>
       <c r="X313">
-        <v>0.273</v>
+        <v>0.275</v>
       </c>
     </row>
     <row r="314" spans="1:24">
@@ -26669,34 +26669,34 @@
         <v>894</v>
       </c>
       <c r="O318">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P318">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="Q318">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="R318">
         <v>6</v>
       </c>
       <c r="S318">
-        <v>-5.2</v>
+        <v>-5.5</v>
       </c>
       <c r="T318">
-        <v>0.064</v>
+        <v>0.06900000000000001</v>
       </c>
       <c r="U318">
-        <v>0.238</v>
+        <v>0.236</v>
       </c>
       <c r="V318">
-        <v>0.154</v>
+        <v>0.161</v>
       </c>
       <c r="W318">
-        <v>0.5669999999999999</v>
+        <v>0.575</v>
       </c>
       <c r="X318">
-        <v>0.115</v>
+        <v>0.107</v>
       </c>
     </row>
     <row r="319" spans="1:24">
@@ -26817,31 +26817,31 @@
         <v>885</v>
       </c>
       <c r="O320">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P320">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="Q320">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="R320">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="S320">
-        <v>5.3</v>
+        <v>6.2</v>
       </c>
       <c r="T320">
         <v>0.03</v>
       </c>
       <c r="U320">
-        <v>0.108</v>
+        <v>0.112</v>
       </c>
       <c r="V320">
-        <v>0.138</v>
+        <v>0.137</v>
       </c>
       <c r="W320">
-        <v>0.499</v>
+        <v>0.505</v>
       </c>
       <c r="X320">
         <v>0.16</v>
@@ -26891,34 +26891,34 @@
         <v>877</v>
       </c>
       <c r="O321">
+        <v>34</v>
+      </c>
+      <c r="P321">
+        <v>153</v>
+      </c>
+      <c r="Q321">
+        <v>80</v>
+      </c>
+      <c r="R321">
         <v>33</v>
       </c>
-      <c r="P321">
-        <v>144</v>
-      </c>
-      <c r="Q321">
-        <v>76</v>
-      </c>
-      <c r="R321">
-        <v>32</v>
-      </c>
       <c r="S321">
-        <v>-7.8</v>
+        <v>-8.1</v>
       </c>
       <c r="T321">
-        <v>0.068</v>
+        <v>0.06900000000000001</v>
       </c>
       <c r="U321">
-        <v>0.08500000000000001</v>
+        <v>0.083</v>
       </c>
       <c r="V321">
-        <v>0.133</v>
+        <v>0.135</v>
       </c>
       <c r="W321">
-        <v>0.526</v>
+        <v>0.52</v>
       </c>
       <c r="X321">
-        <v>0.096</v>
+        <v>0.094</v>
       </c>
     </row>
     <row r="322" spans="1:24">
@@ -27187,34 +27187,34 @@
         <v>900</v>
       </c>
       <c r="O325">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P325">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="Q325">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="R325">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="S325">
-        <v>-19.5</v>
+        <v>-20.1</v>
       </c>
       <c r="T325">
-        <v>0.019</v>
+        <v>0.023</v>
       </c>
       <c r="U325">
-        <v>0.165</v>
+        <v>0.163</v>
       </c>
       <c r="V325">
-        <v>0.259</v>
+        <v>0.253</v>
       </c>
       <c r="W325">
-        <v>0.484</v>
+        <v>0.483</v>
       </c>
       <c r="X325">
-        <v>0.14</v>
+        <v>0.145</v>
       </c>
     </row>
     <row r="326" spans="1:24">
@@ -27409,19 +27409,19 @@
         <v>890</v>
       </c>
       <c r="O328">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P328">
-        <v>238</v>
+        <v>262</v>
       </c>
       <c r="Q328">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="R328">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="S328">
-        <v>-11.3</v>
+        <v>-10.5</v>
       </c>
       <c r="T328">
         <v>0.031</v>
@@ -27430,13 +27430,13 @@
         <v>0.112</v>
       </c>
       <c r="V328">
-        <v>0.149</v>
+        <v>0.15</v>
       </c>
       <c r="W328">
-        <v>0.449</v>
+        <v>0.474</v>
       </c>
       <c r="X328">
-        <v>0.12</v>
+        <v>0.121</v>
       </c>
     </row>
     <row r="329" spans="1:24">
@@ -28223,34 +28223,34 @@
         <v>852</v>
       </c>
       <c r="O339">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P339">
-        <v>368</v>
+        <v>390</v>
       </c>
       <c r="Q339">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="R339">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="S339">
-        <v>13.9</v>
+        <v>14.1</v>
       </c>
       <c r="T339">
-        <v>0.046</v>
+        <v>0.045</v>
       </c>
       <c r="U339">
         <v>0.094</v>
       </c>
       <c r="V339">
-        <v>0.134</v>
+        <v>0.136</v>
       </c>
       <c r="W339">
-        <v>0.5590000000000001</v>
+        <v>0.573</v>
       </c>
       <c r="X339">
-        <v>0.068</v>
+        <v>0.06900000000000001</v>
       </c>
     </row>
     <row r="340" spans="1:24">
@@ -28963,13 +28963,13 @@
         <v>902</v>
       </c>
       <c r="O349">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P349">
-        <v>659</v>
+        <v>662</v>
       </c>
       <c r="Q349">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="R349">
         <v>76</v>
@@ -28978,19 +28978,19 @@
         <v>1.6</v>
       </c>
       <c r="T349">
-        <v>0.019</v>
+        <v>0.018</v>
       </c>
       <c r="U349">
         <v>0.08400000000000001</v>
       </c>
       <c r="V349">
-        <v>0.22</v>
+        <v>0.219</v>
       </c>
       <c r="W349">
-        <v>0.577</v>
+        <v>0.569</v>
       </c>
       <c r="X349">
-        <v>0.102</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="350" spans="1:24">
@@ -29037,34 +29037,34 @@
         <v>914</v>
       </c>
       <c r="O350">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P350">
-        <v>550</v>
+        <v>576</v>
       </c>
       <c r="Q350">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="R350">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="S350">
-        <v>5</v>
+        <v>5.3</v>
       </c>
       <c r="T350">
-        <v>0.01</v>
+        <v>0.011</v>
       </c>
       <c r="U350">
-        <v>0.108</v>
+        <v>0.106</v>
       </c>
       <c r="V350">
         <v>0.226</v>
       </c>
       <c r="W350">
-        <v>0.5600000000000001</v>
+        <v>0.5620000000000001</v>
       </c>
       <c r="X350">
-        <v>0.245</v>
+        <v>0.248</v>
       </c>
     </row>
     <row r="351" spans="1:24">
@@ -29185,34 +29185,34 @@
         <v>897</v>
       </c>
       <c r="O352">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="P352">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="Q352">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="R352">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="S352">
-        <v>-2.5</v>
+        <v>-1.8</v>
       </c>
       <c r="T352">
-        <v>0.025</v>
+        <v>0.024</v>
       </c>
       <c r="U352">
-        <v>0.049</v>
+        <v>0.052</v>
       </c>
       <c r="V352">
-        <v>0.172</v>
+        <v>0.171</v>
       </c>
       <c r="W352">
         <v>0.594</v>
       </c>
       <c r="X352">
-        <v>0.216</v>
+        <v>0.223</v>
       </c>
     </row>
     <row r="353" spans="1:24">
@@ -29629,34 +29629,34 @@
         <v>898</v>
       </c>
       <c r="O358">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P358">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="Q358">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="R358">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="S358">
-        <v>0.6</v>
+        <v>1.1</v>
       </c>
       <c r="T358">
-        <v>0.094</v>
+        <v>0.096</v>
       </c>
       <c r="U358">
-        <v>0.253</v>
+        <v>0.256</v>
       </c>
       <c r="V358">
         <v>0.103</v>
       </c>
       <c r="W358">
-        <v>0.588</v>
+        <v>0.597</v>
       </c>
       <c r="X358">
-        <v>0.138</v>
+        <v>0.141</v>
       </c>
     </row>
     <row r="359" spans="1:24">
@@ -29925,34 +29925,34 @@
         <v>852</v>
       </c>
       <c r="O362">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P362">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="Q362">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="R362">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S362">
-        <v>5.3</v>
+        <v>-0.4</v>
       </c>
       <c r="T362">
-        <v>0.036</v>
+        <v>0.033</v>
       </c>
       <c r="U362">
-        <v>0.113</v>
+        <v>0.116</v>
       </c>
       <c r="V362">
         <v>0.145</v>
       </c>
       <c r="W362">
-        <v>0.591</v>
+        <v>0.58</v>
       </c>
       <c r="X362">
-        <v>0.167</v>
+        <v>0.163</v>
       </c>
     </row>
     <row r="363" spans="1:24">
@@ -30591,34 +30591,34 @@
         <v>891</v>
       </c>
       <c r="O371">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P371">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="Q371">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="R371">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="S371">
-        <v>-6.8</v>
+        <v>-6.1</v>
       </c>
       <c r="T371">
-        <v>0.067</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="U371">
-        <v>0.273</v>
+        <v>0.269</v>
       </c>
       <c r="V371">
-        <v>0.157</v>
+        <v>0.155</v>
       </c>
       <c r="W371">
-        <v>0.52</v>
+        <v>0.525</v>
       </c>
       <c r="X371">
-        <v>0.074</v>
+        <v>0.075</v>
       </c>
     </row>
     <row r="372" spans="1:24">
@@ -30665,22 +30665,22 @@
         <v>903</v>
       </c>
       <c r="O372">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P372">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="Q372">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="R372">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="S372">
-        <v>5.7</v>
+        <v>4.4</v>
       </c>
       <c r="T372">
-        <v>0.021</v>
+        <v>0.022</v>
       </c>
       <c r="U372">
         <v>0.09</v>
@@ -30689,10 +30689,10 @@
         <v>0.165</v>
       </c>
       <c r="W372">
-        <v>0.539</v>
+        <v>0.538</v>
       </c>
       <c r="X372">
-        <v>0.173</v>
+        <v>0.188</v>
       </c>
     </row>
     <row r="373" spans="1:24">
@@ -31109,34 +31109,34 @@
         <v>914</v>
       </c>
       <c r="O378">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P378">
-        <v>572</v>
+        <v>600</v>
       </c>
       <c r="Q378">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="R378">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="S378">
-        <v>1.4</v>
+        <v>1.9</v>
       </c>
       <c r="T378">
-        <v>0.048</v>
+        <v>0.047</v>
       </c>
       <c r="U378">
-        <v>0.177</v>
+        <v>0.174</v>
       </c>
       <c r="V378">
         <v>0.205</v>
       </c>
       <c r="W378">
-        <v>0.6</v>
+        <v>0.608</v>
       </c>
       <c r="X378">
-        <v>0.07099999999999999</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="379" spans="1:24">
@@ -31775,34 +31775,34 @@
         <v>897</v>
       </c>
       <c r="O387">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P387">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="Q387">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="R387">
         <v>57</v>
       </c>
       <c r="S387">
-        <v>5.4</v>
+        <v>5.6</v>
       </c>
       <c r="T387">
-        <v>0.036</v>
+        <v>0.035</v>
       </c>
       <c r="U387">
-        <v>0.11</v>
+        <v>0.112</v>
       </c>
       <c r="V387">
-        <v>0.083</v>
+        <v>0.082</v>
       </c>
       <c r="W387">
-        <v>0.539</v>
+        <v>0.548</v>
       </c>
       <c r="X387">
-        <v>0.108</v>
+        <v>0.106</v>
       </c>
     </row>
     <row r="388" spans="1:24">
@@ -32145,34 +32145,34 @@
         <v>911</v>
       </c>
       <c r="O392">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P392">
-        <v>759</v>
+        <v>782</v>
       </c>
       <c r="Q392">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="R392">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="S392">
-        <v>5</v>
+        <v>6.1</v>
       </c>
       <c r="T392">
-        <v>0.01</v>
+        <v>0.011</v>
       </c>
       <c r="U392">
-        <v>0.092</v>
+        <v>0.093</v>
       </c>
       <c r="V392">
         <v>0.27</v>
       </c>
       <c r="W392">
-        <v>0.635</v>
+        <v>0.637</v>
       </c>
       <c r="X392">
-        <v>0.111</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="393" spans="1:24">
@@ -32293,34 +32293,34 @@
         <v>918</v>
       </c>
       <c r="O394">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P394">
-        <v>390</v>
+        <v>397</v>
       </c>
       <c r="Q394">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="R394">
         <v>63</v>
       </c>
       <c r="S394">
-        <v>-2.9</v>
+        <v>-3.4</v>
       </c>
       <c r="T394">
-        <v>0.035</v>
+        <v>0.036</v>
       </c>
       <c r="U394">
         <v>0.164</v>
       </c>
       <c r="V394">
-        <v>0.178</v>
+        <v>0.179</v>
       </c>
       <c r="W394">
-        <v>0.65</v>
+        <v>0.647</v>
       </c>
       <c r="X394">
-        <v>0.116</v>
+        <v>0.114</v>
       </c>
     </row>
     <row r="395" spans="1:24">
@@ -32737,34 +32737,34 @@
         <v>909</v>
       </c>
       <c r="O400">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P400">
         <v>134</v>
       </c>
       <c r="Q400">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="R400">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S400">
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
       <c r="T400">
-        <v>0.065</v>
+        <v>0.063</v>
       </c>
       <c r="U400">
-        <v>0.154</v>
+        <v>0.153</v>
       </c>
       <c r="V400">
-        <v>0.108</v>
+        <v>0.106</v>
       </c>
       <c r="W400">
-        <v>0.59</v>
+        <v>0.579</v>
       </c>
       <c r="X400">
-        <v>0.083</v>
+        <v>0.082</v>
       </c>
     </row>
     <row r="401" spans="1:24">
@@ -32811,34 +32811,34 @@
         <v>914</v>
       </c>
       <c r="O401">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="P401">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="Q401">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="R401">
         <v>14</v>
       </c>
       <c r="S401">
-        <v>4.1</v>
+        <v>2</v>
       </c>
       <c r="T401">
-        <v>0.039</v>
+        <v>0.041</v>
       </c>
       <c r="U401">
-        <v>0.175</v>
+        <v>0.17</v>
       </c>
       <c r="V401">
-        <v>0.151</v>
+        <v>0.152</v>
       </c>
       <c r="W401">
-        <v>0.415</v>
+        <v>0.414</v>
       </c>
       <c r="X401">
-        <v>0.093</v>
+        <v>0.091</v>
       </c>
     </row>
     <row r="402" spans="1:24">
@@ -33255,34 +33255,34 @@
         <v>900</v>
       </c>
       <c r="O407">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P407">
-        <v>819</v>
+        <v>845</v>
       </c>
       <c r="Q407">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="R407">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="S407">
-        <v>2.8</v>
+        <v>3.2</v>
       </c>
       <c r="T407">
-        <v>0.053</v>
+        <v>0.051</v>
       </c>
       <c r="U407">
         <v>0.165</v>
       </c>
       <c r="V407">
-        <v>0.226</v>
+        <v>0.227</v>
       </c>
       <c r="W407">
-        <v>0.611</v>
+        <v>0.609</v>
       </c>
       <c r="X407">
-        <v>0.15</v>
+        <v>0.153</v>
       </c>
     </row>
     <row r="408" spans="1:24">
@@ -34661,34 +34661,34 @@
         <v>926</v>
       </c>
       <c r="O426">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P426">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="Q426">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="R426">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="S426">
-        <v>-11.9</v>
+        <v>-11.4</v>
       </c>
       <c r="T426">
-        <v>0.058</v>
+        <v>0.063</v>
       </c>
       <c r="U426">
-        <v>0.077</v>
+        <v>0.074</v>
       </c>
       <c r="V426">
-        <v>0.138</v>
+        <v>0.14</v>
       </c>
       <c r="W426">
-        <v>0.506</v>
+        <v>0.518</v>
       </c>
       <c r="X426">
-        <v>0.075</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="427" spans="1:24">
@@ -35253,34 +35253,34 @@
         <v>900</v>
       </c>
       <c r="O434">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="P434">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="Q434">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="R434">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="S434">
-        <v>-5.7</v>
+        <v>-5.6</v>
       </c>
       <c r="T434">
-        <v>0.098</v>
+        <v>0.096</v>
       </c>
       <c r="U434">
-        <v>0.192</v>
+        <v>0.199</v>
       </c>
       <c r="V434">
-        <v>0.124</v>
+        <v>0.125</v>
       </c>
       <c r="W434">
-        <v>0.764</v>
+        <v>0.746</v>
       </c>
       <c r="X434">
-        <v>0.094</v>
+        <v>0.101</v>
       </c>
     </row>
     <row r="435" spans="1:24">
@@ -35327,10 +35327,10 @@
         <v>885</v>
       </c>
       <c r="O435">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P435">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="Q435">
         <v>115</v>
@@ -35339,22 +35339,22 @@
         <v>31</v>
       </c>
       <c r="S435">
-        <v>-3.6</v>
+        <v>-4</v>
       </c>
       <c r="T435">
-        <v>0.032</v>
+        <v>0.031</v>
       </c>
       <c r="U435">
-        <v>0.149</v>
+        <v>0.147</v>
       </c>
       <c r="V435">
-        <v>0.173</v>
+        <v>0.175</v>
       </c>
       <c r="W435">
-        <v>0.5570000000000001</v>
+        <v>0.553</v>
       </c>
       <c r="X435">
-        <v>0.073</v>
+        <v>0.07199999999999999</v>
       </c>
     </row>
     <row r="436" spans="1:24">
@@ -35401,31 +35401,31 @@
         <v>852</v>
       </c>
       <c r="O436">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P436">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="Q436">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="R436">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="S436">
-        <v>-0.8</v>
+        <v>-1</v>
       </c>
       <c r="T436">
-        <v>0.037</v>
+        <v>0.036</v>
       </c>
       <c r="U436">
         <v>0.169</v>
       </c>
       <c r="V436">
-        <v>0.157</v>
+        <v>0.156</v>
       </c>
       <c r="W436">
-        <v>0.601</v>
+        <v>0.604</v>
       </c>
       <c r="X436">
         <v>0.132</v>
@@ -35697,31 +35697,31 @@
         <v>905</v>
       </c>
       <c r="O440">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P440">
-        <v>251</v>
+        <v>269</v>
       </c>
       <c r="Q440">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="R440">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="S440">
-        <v>-2.3</v>
+        <v>-1.7</v>
       </c>
       <c r="T440">
-        <v>0.044</v>
+        <v>0.045</v>
       </c>
       <c r="U440">
-        <v>0.105</v>
+        <v>0.111</v>
       </c>
       <c r="V440">
-        <v>0.148</v>
+        <v>0.15</v>
       </c>
       <c r="W440">
-        <v>0.545</v>
+        <v>0.555</v>
       </c>
       <c r="X440">
         <v>0.065</v>
@@ -35919,34 +35919,34 @@
         <v>932</v>
       </c>
       <c r="O443">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P443">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="Q443">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="R443">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S443">
-        <v>9.5</v>
+        <v>10.6</v>
       </c>
       <c r="T443">
         <v>0.019</v>
       </c>
       <c r="U443">
-        <v>0.07000000000000001</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="V443">
-        <v>0.149</v>
+        <v>0.15</v>
       </c>
       <c r="W443">
-        <v>0.544</v>
+        <v>0.55</v>
       </c>
       <c r="X443">
-        <v>0.115</v>
+        <v>0.119</v>
       </c>
     </row>
     <row r="444" spans="1:24">
@@ -36141,34 +36141,34 @@
         <v>883</v>
       </c>
       <c r="O446">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P446">
-        <v>378</v>
+        <v>394</v>
       </c>
       <c r="Q446">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="R446">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="S446">
-        <v>-9.1</v>
+        <v>-9.800000000000001</v>
       </c>
       <c r="T446">
-        <v>0.024</v>
+        <v>0.023</v>
       </c>
       <c r="U446">
-        <v>0.08500000000000001</v>
+        <v>0.08400000000000001</v>
       </c>
       <c r="V446">
-        <v>0.216</v>
+        <v>0.217</v>
       </c>
       <c r="W446">
-        <v>0.53</v>
+        <v>0.531</v>
       </c>
       <c r="X446">
-        <v>0.276</v>
+        <v>0.277</v>
       </c>
     </row>
     <row r="447" spans="1:24">
@@ -36437,22 +36437,22 @@
         <v>896</v>
       </c>
       <c r="O450">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P450">
-        <v>569</v>
+        <v>581</v>
       </c>
       <c r="Q450">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="R450">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="S450">
-        <v>-8.300000000000001</v>
+        <v>-9.199999999999999</v>
       </c>
       <c r="T450">
-        <v>0.02</v>
+        <v>0.021</v>
       </c>
       <c r="U450">
         <v>0.1</v>
@@ -36464,7 +36464,7 @@
         <v>0.553</v>
       </c>
       <c r="X450">
-        <v>0.133</v>
+        <v>0.137</v>
       </c>
     </row>
     <row r="451" spans="1:24">
@@ -36511,34 +36511,34 @@
         <v>914</v>
       </c>
       <c r="O451">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P451">
-        <v>1224</v>
+        <v>1264</v>
       </c>
       <c r="Q451">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="R451">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="S451">
-        <v>17.6</v>
+        <v>18.4</v>
       </c>
       <c r="T451">
-        <v>0.024</v>
+        <v>0.023</v>
       </c>
       <c r="U451">
-        <v>0.124</v>
+        <v>0.123</v>
       </c>
       <c r="V451">
-        <v>0.327</v>
+        <v>0.329</v>
       </c>
       <c r="W451">
-        <v>0.64</v>
+        <v>0.642</v>
       </c>
       <c r="X451">
-        <v>0.284</v>
+        <v>0.287</v>
       </c>
     </row>
     <row r="452" spans="1:24">
@@ -36733,34 +36733,34 @@
         <v>852</v>
       </c>
       <c r="O454">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P454">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="Q454">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="R454">
         <v>31</v>
       </c>
       <c r="S454">
-        <v>-2.9</v>
+        <v>-3.2</v>
       </c>
       <c r="T454">
         <v>0.037</v>
       </c>
       <c r="U454">
-        <v>0.127</v>
+        <v>0.124</v>
       </c>
       <c r="V454">
-        <v>0.154</v>
+        <v>0.153</v>
       </c>
       <c r="W454">
-        <v>0.5610000000000001</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="X454">
-        <v>0.068</v>
+        <v>0.066</v>
       </c>
     </row>
     <row r="455" spans="1:24">
@@ -37177,31 +37177,31 @@
         <v>884</v>
       </c>
       <c r="O460">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P460">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="Q460">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="R460">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="S460">
-        <v>6.8</v>
+        <v>8.9</v>
       </c>
       <c r="T460">
-        <v>0.187</v>
+        <v>0.183</v>
       </c>
       <c r="U460">
-        <v>0.205</v>
+        <v>0.207</v>
       </c>
       <c r="V460">
-        <v>0.128</v>
+        <v>0.126</v>
       </c>
       <c r="W460">
-        <v>0.5580000000000001</v>
+        <v>0.572</v>
       </c>
       <c r="X460">
         <v>0.124</v>
@@ -37322,34 +37322,34 @@
         <v>876</v>
       </c>
       <c r="O462">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P462">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="Q462">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="R462">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="S462">
-        <v>-4.5</v>
+        <v>-4.4</v>
       </c>
       <c r="T462">
-        <v>0.031</v>
+        <v>0.03</v>
       </c>
       <c r="U462">
-        <v>0.1</v>
+        <v>0.103</v>
       </c>
       <c r="V462">
-        <v>0.231</v>
+        <v>0.23</v>
       </c>
       <c r="W462">
-        <v>0.5629999999999999</v>
+        <v>0.556</v>
       </c>
       <c r="X462">
-        <v>0.328</v>
+        <v>0.332</v>
       </c>
     </row>
     <row r="463" spans="1:24">
@@ -37544,34 +37544,34 @@
         <v>921</v>
       </c>
       <c r="O465">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P465">
-        <v>270</v>
+        <v>286</v>
       </c>
       <c r="Q465">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="R465">
         <v>25</v>
       </c>
       <c r="S465">
-        <v>8.699999999999999</v>
+        <v>8.1</v>
       </c>
       <c r="T465">
-        <v>0.083</v>
+        <v>0.081</v>
       </c>
       <c r="U465">
-        <v>0.165</v>
+        <v>0.164</v>
       </c>
       <c r="V465">
         <v>0.189</v>
       </c>
       <c r="W465">
-        <v>0.5570000000000001</v>
+        <v>0.5610000000000001</v>
       </c>
       <c r="X465">
-        <v>0.067</v>
+        <v>0.064</v>
       </c>
     </row>
     <row r="466" spans="1:24">
@@ -37840,34 +37840,34 @@
         <v>925</v>
       </c>
       <c r="O469">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P469">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="Q469">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="R469">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="S469">
-        <v>-3.8</v>
+        <v>-3.5</v>
       </c>
       <c r="T469">
-        <v>0.045</v>
+        <v>0.044</v>
       </c>
       <c r="U469">
-        <v>0.101</v>
+        <v>0.106</v>
       </c>
       <c r="V469">
-        <v>0.134</v>
+        <v>0.136</v>
       </c>
       <c r="W469">
-        <v>0.547</v>
+        <v>0.5610000000000001</v>
       </c>
       <c r="X469">
-        <v>0.117</v>
+        <v>0.115</v>
       </c>
     </row>
     <row r="470" spans="1:24">
@@ -38062,34 +38062,34 @@
         <v>907</v>
       </c>
       <c r="O472">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P472">
         <v>143</v>
       </c>
       <c r="Q472">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="R472">
         <v>17</v>
       </c>
       <c r="S472">
-        <v>6.6</v>
+        <v>5.3</v>
       </c>
       <c r="T472">
-        <v>0.08699999999999999</v>
+        <v>0.089</v>
       </c>
       <c r="U472">
-        <v>0.17</v>
+        <v>0.173</v>
       </c>
       <c r="V472">
-        <v>0.145</v>
+        <v>0.146</v>
       </c>
       <c r="W472">
-        <v>0.675</v>
+        <v>0.65</v>
       </c>
       <c r="X472">
-        <v>0.07099999999999999</v>
+        <v>0.06900000000000001</v>
       </c>
     </row>
     <row r="473" spans="1:24">
@@ -38210,34 +38210,34 @@
         <v>890</v>
       </c>
       <c r="O474">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P474">
-        <v>393</v>
+        <v>418</v>
       </c>
       <c r="Q474">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="R474">
         <v>57</v>
       </c>
       <c r="S474">
-        <v>-4.8</v>
+        <v>-5.1</v>
       </c>
       <c r="T474">
         <v>0.007</v>
       </c>
       <c r="U474">
-        <v>0.066</v>
+        <v>0.068</v>
       </c>
       <c r="V474">
-        <v>0.148</v>
+        <v>0.152</v>
       </c>
       <c r="W474">
-        <v>0.589</v>
+        <v>0.593</v>
       </c>
       <c r="X474">
-        <v>0.076</v>
+        <v>0.074</v>
       </c>
     </row>
     <row r="475" spans="1:24">
@@ -38284,31 +38284,31 @@
         <v>902</v>
       </c>
       <c r="O475">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P475">
-        <v>506</v>
+        <v>516</v>
       </c>
       <c r="Q475">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="R475">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="S475">
         <v>2.3</v>
       </c>
       <c r="T475">
-        <v>0.032</v>
+        <v>0.031</v>
       </c>
       <c r="U475">
-        <v>0.168</v>
+        <v>0.166</v>
       </c>
       <c r="V475">
-        <v>0.175</v>
+        <v>0.174</v>
       </c>
       <c r="W475">
-        <v>0.553</v>
+        <v>0.55</v>
       </c>
       <c r="X475">
         <v>0.108</v>
@@ -38506,34 +38506,34 @@
         <v>930</v>
       </c>
       <c r="O478">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P478">
         <v>374</v>
       </c>
       <c r="Q478">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="R478">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="S478">
-        <v>-8.6</v>
+        <v>-9.4</v>
       </c>
       <c r="T478">
-        <v>0.06900000000000001</v>
+        <v>0.067</v>
       </c>
       <c r="U478">
-        <v>0.104</v>
+        <v>0.103</v>
       </c>
       <c r="V478">
-        <v>0.141</v>
+        <v>0.14</v>
       </c>
       <c r="W478">
-        <v>0.538</v>
+        <v>0.53</v>
       </c>
       <c r="X478">
-        <v>0.08799999999999999</v>
+        <v>0.089</v>
       </c>
     </row>
     <row r="479" spans="1:24">
@@ -39139,10 +39139,10 @@
         <v>508</v>
       </c>
       <c r="D487">
-        <v>1610612740</v>
+        <v>1610612747</v>
       </c>
       <c r="E487" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="F487">
         <v>25</v>
@@ -39246,34 +39246,34 @@
         <v>884</v>
       </c>
       <c r="O488">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P488">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="Q488">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="R488">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="S488">
-        <v>4.1</v>
+        <v>3.8</v>
       </c>
       <c r="T488">
-        <v>0.053</v>
+        <v>0.051</v>
       </c>
       <c r="U488">
-        <v>0.17</v>
+        <v>0.172</v>
       </c>
       <c r="V488">
-        <v>0.139</v>
+        <v>0.14</v>
       </c>
       <c r="W488">
-        <v>0.556</v>
+        <v>0.546</v>
       </c>
       <c r="X488">
-        <v>0.062</v>
+        <v>0.064</v>
       </c>
     </row>
     <row r="489" spans="1:24">
@@ -39394,34 +39394,34 @@
         <v>878</v>
       </c>
       <c r="O490">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P490">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="Q490">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="R490">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="S490">
-        <v>-22</v>
+        <v>-12.8</v>
       </c>
       <c r="T490">
-        <v>0.08</v>
+        <v>0.079</v>
       </c>
       <c r="U490">
-        <v>0.233</v>
+        <v>0.239</v>
       </c>
       <c r="V490">
-        <v>0.179</v>
+        <v>0.169</v>
       </c>
       <c r="W490">
-        <v>0.461</v>
+        <v>0.476</v>
       </c>
       <c r="X490">
-        <v>0.07000000000000001</v>
+        <v>0.08799999999999999</v>
       </c>
     </row>
     <row r="491" spans="1:24">
@@ -39690,34 +39690,34 @@
         <v>890</v>
       </c>
       <c r="O494">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P494">
-        <v>363</v>
+        <v>375</v>
       </c>
       <c r="Q494">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="R494">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="S494">
-        <v>7.7</v>
+        <v>7.8</v>
       </c>
       <c r="T494">
-        <v>0.038</v>
+        <v>0.039</v>
       </c>
       <c r="U494">
-        <v>0.083</v>
+        <v>0.08400000000000001</v>
       </c>
       <c r="V494">
-        <v>0.217</v>
+        <v>0.215</v>
       </c>
       <c r="W494">
-        <v>0.625</v>
+        <v>0.633</v>
       </c>
       <c r="X494">
-        <v>0.266</v>
+        <v>0.268</v>
       </c>
     </row>
     <row r="495" spans="1:24">
@@ -40060,34 +40060,34 @@
         <v>884</v>
       </c>
       <c r="O499">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P499">
-        <v>725</v>
+        <v>742</v>
       </c>
       <c r="Q499">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="R499">
-        <v>353</v>
+        <v>361</v>
       </c>
       <c r="S499">
-        <v>1.6</v>
+        <v>1.9</v>
       </c>
       <c r="T499">
         <v>0.019</v>
       </c>
       <c r="U499">
-        <v>0.083</v>
+        <v>0.08400000000000001</v>
       </c>
       <c r="V499">
-        <v>0.21</v>
+        <v>0.209</v>
       </c>
       <c r="W499">
-        <v>0.59</v>
+        <v>0.589</v>
       </c>
       <c r="X499">
-        <v>0.359</v>
+        <v>0.358</v>
       </c>
     </row>
     <row r="500" spans="1:24">
@@ -40282,34 +40282,34 @@
         <v>890</v>
       </c>
       <c r="O502">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P502">
-        <v>439</v>
+        <v>448</v>
       </c>
       <c r="Q502">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="R502">
-        <v>228</v>
+        <v>238</v>
       </c>
       <c r="S502">
-        <v>-3.9</v>
+        <v>-3.2</v>
       </c>
       <c r="T502">
         <v>0.019</v>
       </c>
       <c r="U502">
-        <v>0.063</v>
+        <v>0.062</v>
       </c>
       <c r="V502">
-        <v>0.157</v>
+        <v>0.156</v>
       </c>
       <c r="W502">
         <v>0.604</v>
       </c>
       <c r="X502">
-        <v>0.285</v>
+        <v>0.288</v>
       </c>
     </row>
     <row r="503" spans="1:24">

</xml_diff>

<commit_message>
New model w/ new features, fixed some fundamental methods
Added a new model with new features which currently has less accuracy than the current one but with further data I think it will be better. Also changed the way a few methods worked so we could finally add names with Jr. so I added Michael Porter Jr. and Jaren Jackson Jr.
</commit_message>
<xml_diff>
--- a/Players_Data.xlsx
+++ b/Players_Data.xlsx
@@ -6032,31 +6032,31 @@
         <v>879</v>
       </c>
       <c r="O39">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P39">
-        <v>622</v>
+        <v>628</v>
       </c>
       <c r="Q39">
-        <v>377</v>
+        <v>388</v>
       </c>
       <c r="R39">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="S39">
-        <v>-0.5</v>
+        <v>0.2</v>
       </c>
       <c r="T39">
-        <v>0.067</v>
+        <v>0.068</v>
       </c>
       <c r="U39">
-        <v>0.219</v>
+        <v>0.22</v>
       </c>
       <c r="V39">
-        <v>0.224</v>
+        <v>0.223</v>
       </c>
       <c r="W39">
-        <v>0.523</v>
+        <v>0.52</v>
       </c>
       <c r="X39">
         <v>0.216</v>
@@ -6476,34 +6476,34 @@
         <v>897</v>
       </c>
       <c r="O45">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P45">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="Q45">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="R45">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="S45">
-        <v>4.5</v>
+        <v>4.8</v>
       </c>
       <c r="T45">
         <v>0.024</v>
       </c>
       <c r="U45">
-        <v>0.055</v>
+        <v>0.058</v>
       </c>
       <c r="V45">
-        <v>0.178</v>
+        <v>0.181</v>
       </c>
       <c r="W45">
-        <v>0.51</v>
+        <v>0.516</v>
       </c>
       <c r="X45">
-        <v>0.249</v>
+        <v>0.256</v>
       </c>
     </row>
     <row r="46" spans="1:24">
@@ -9066,34 +9066,34 @@
         <v>912</v>
       </c>
       <c r="O80">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P80">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="Q80">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="R80">
         <v>12</v>
       </c>
       <c r="S80">
-        <v>-11.3</v>
+        <v>-11.8</v>
       </c>
       <c r="T80">
-        <v>0.136</v>
+        <v>0.133</v>
       </c>
       <c r="U80">
-        <v>0.237</v>
+        <v>0.242</v>
       </c>
       <c r="V80">
-        <v>0.171</v>
+        <v>0.168</v>
       </c>
       <c r="W80">
-        <v>0.601</v>
+        <v>0.599</v>
       </c>
       <c r="X80">
-        <v>0.063</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="81" spans="1:24">
@@ -9436,34 +9436,34 @@
         <v>878</v>
       </c>
       <c r="O85">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P85">
-        <v>383</v>
+        <v>393</v>
       </c>
       <c r="Q85">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="R85">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="S85">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="T85">
-        <v>0.017</v>
+        <v>0.016</v>
       </c>
       <c r="U85">
         <v>0.119</v>
       </c>
       <c r="V85">
-        <v>0.142</v>
+        <v>0.141</v>
       </c>
       <c r="W85">
-        <v>0.576</v>
+        <v>0.58</v>
       </c>
       <c r="X85">
-        <v>0.376</v>
+        <v>0.378</v>
       </c>
     </row>
     <row r="86" spans="1:24">
@@ -13432,34 +13432,34 @@
         <v>914</v>
       </c>
       <c r="O139">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P139">
-        <v>400</v>
+        <v>423</v>
       </c>
       <c r="Q139">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="R139">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="S139">
-        <v>-9.800000000000001</v>
+        <v>-11</v>
       </c>
       <c r="T139">
-        <v>0.026</v>
+        <v>0.024</v>
       </c>
       <c r="U139">
         <v>0.094</v>
       </c>
       <c r="V139">
-        <v>0.232</v>
+        <v>0.233</v>
       </c>
       <c r="W139">
         <v>0.545</v>
       </c>
       <c r="X139">
-        <v>0.173</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="140" spans="1:24">
@@ -14468,34 +14468,34 @@
         <v>852</v>
       </c>
       <c r="O153">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P153">
-        <v>397</v>
+        <v>418</v>
       </c>
       <c r="Q153">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="R153">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="S153">
-        <v>1</v>
+        <v>1.9</v>
       </c>
       <c r="T153">
-        <v>0.013</v>
+        <v>0.014</v>
       </c>
       <c r="U153">
-        <v>0.08599999999999999</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="V153">
         <v>0.195</v>
       </c>
       <c r="W153">
-        <v>0.5620000000000001</v>
+        <v>0.572</v>
       </c>
       <c r="X153">
-        <v>0.175</v>
+        <v>0.172</v>
       </c>
     </row>
     <row r="154" spans="1:24">
@@ -16392,34 +16392,34 @@
         <v>896</v>
       </c>
       <c r="O179">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P179">
-        <v>447</v>
+        <v>457</v>
       </c>
       <c r="Q179">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="R179">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="S179">
-        <v>0.7</v>
+        <v>0.1</v>
       </c>
       <c r="T179">
         <v>0.048</v>
       </c>
       <c r="U179">
-        <v>0.078</v>
+        <v>0.079</v>
       </c>
       <c r="V179">
         <v>0.144</v>
       </c>
       <c r="W179">
-        <v>0.627</v>
+        <v>0.623</v>
       </c>
       <c r="X179">
-        <v>0.08400000000000001</v>
+        <v>0.08500000000000001</v>
       </c>
     </row>
     <row r="180" spans="1:24">
@@ -16534,34 +16534,34 @@
         <v>855</v>
       </c>
       <c r="O181">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P181">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="Q181">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="R181">
         <v>48</v>
       </c>
       <c r="S181">
-        <v>-2</v>
+        <v>-2.4</v>
       </c>
       <c r="T181">
-        <v>0.033</v>
+        <v>0.035</v>
       </c>
       <c r="U181">
         <v>0.094</v>
       </c>
       <c r="V181">
-        <v>0.111</v>
+        <v>0.112</v>
       </c>
       <c r="W181">
-        <v>0.614</v>
+        <v>0.611</v>
       </c>
       <c r="X181">
-        <v>0.07099999999999999</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="182" spans="1:24">
@@ -18606,34 +18606,34 @@
         <v>920</v>
       </c>
       <c r="O209">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P209">
-        <v>344</v>
+        <v>356</v>
       </c>
       <c r="Q209">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="R209">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="S209">
-        <v>-6.2</v>
+        <v>-6</v>
       </c>
       <c r="T209">
-        <v>0.051</v>
+        <v>0.052</v>
       </c>
       <c r="U209">
-        <v>0.14</v>
+        <v>0.141</v>
       </c>
       <c r="V209">
-        <v>0.195</v>
+        <v>0.194</v>
       </c>
       <c r="W209">
-        <v>0.526</v>
+        <v>0.533</v>
       </c>
       <c r="X209">
-        <v>0.18</v>
+        <v>0.176</v>
       </c>
     </row>
     <row r="210" spans="1:24">
@@ -22081,34 +22081,34 @@
         <v>894</v>
       </c>
       <c r="O256">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P256">
-        <v>405</v>
+        <v>413</v>
       </c>
       <c r="Q256">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="R256">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="S256">
-        <v>3.3</v>
+        <v>4.4</v>
       </c>
       <c r="T256">
-        <v>0.075</v>
+        <v>0.07199999999999999</v>
       </c>
       <c r="U256">
-        <v>0.103</v>
+        <v>0.102</v>
       </c>
       <c r="V256">
-        <v>0.205</v>
+        <v>0.202</v>
       </c>
       <c r="W256">
-        <v>0.642</v>
+        <v>0.639</v>
       </c>
       <c r="X256">
-        <v>0.226</v>
+        <v>0.229</v>
       </c>
     </row>
     <row r="257" spans="1:24">
@@ -23561,7 +23561,7 @@
         <v>890</v>
       </c>
       <c r="O276">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P276">
         <v>5</v>
@@ -23573,22 +23573,22 @@
         <v>4</v>
       </c>
       <c r="S276">
-        <v>-1.4</v>
+        <v>-5.4</v>
       </c>
       <c r="T276">
         <v>0</v>
       </c>
       <c r="U276">
-        <v>0.091</v>
+        <v>0.083</v>
       </c>
       <c r="V276">
-        <v>0.182</v>
+        <v>0.192</v>
       </c>
       <c r="W276">
-        <v>0.644</v>
+        <v>0.425</v>
       </c>
       <c r="X276">
-        <v>0.235</v>
+        <v>0.211</v>
       </c>
     </row>
     <row r="277" spans="1:24">
@@ -24153,34 +24153,34 @@
         <v>852</v>
       </c>
       <c r="O284">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P284">
-        <v>459</v>
+        <v>464</v>
       </c>
       <c r="Q284">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="R284">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="S284">
-        <v>0</v>
+        <v>-0.3</v>
       </c>
       <c r="T284">
-        <v>0.027</v>
+        <v>0.028</v>
       </c>
       <c r="U284">
-        <v>0.124</v>
+        <v>0.123</v>
       </c>
       <c r="V284">
-        <v>0.168</v>
+        <v>0.167</v>
       </c>
       <c r="W284">
-        <v>0.582</v>
+        <v>0.576</v>
       </c>
       <c r="X284">
-        <v>0.066</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="285" spans="1:24">
@@ -25337,34 +25337,34 @@
         <v>917</v>
       </c>
       <c r="O300">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P300">
-        <v>164</v>
+        <v>189</v>
       </c>
       <c r="Q300">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="R300">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="S300">
-        <v>2.1</v>
+        <v>5.5</v>
       </c>
       <c r="T300">
-        <v>0.06900000000000001</v>
+        <v>0.076</v>
       </c>
       <c r="U300">
-        <v>0.193</v>
+        <v>0.185</v>
       </c>
       <c r="V300">
-        <v>0.181</v>
+        <v>0.189</v>
       </c>
       <c r="W300">
-        <v>0.65</v>
+        <v>0.643</v>
       </c>
       <c r="X300">
-        <v>0.063</v>
+        <v>0.064</v>
       </c>
     </row>
     <row r="301" spans="1:24">
@@ -25411,19 +25411,19 @@
         <v>919</v>
       </c>
       <c r="O301">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P301">
-        <v>460</v>
+        <v>468</v>
       </c>
       <c r="Q301">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="R301">
         <v>55</v>
       </c>
       <c r="S301">
-        <v>-7</v>
+        <v>-7.7</v>
       </c>
       <c r="T301">
         <v>0.048</v>
@@ -25432,13 +25432,13 @@
         <v>0.144</v>
       </c>
       <c r="V301">
-        <v>0.204</v>
+        <v>0.203</v>
       </c>
       <c r="W301">
-        <v>0.553</v>
+        <v>0.551</v>
       </c>
       <c r="X301">
-        <v>0.097</v>
+        <v>0.095</v>
       </c>
     </row>
     <row r="302" spans="1:24">
@@ -25929,25 +25929,25 @@
         <v>852</v>
       </c>
       <c r="O308">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="P308">
         <v>14</v>
       </c>
       <c r="Q308">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="R308">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S308">
-        <v>4.6</v>
+        <v>2.6</v>
       </c>
       <c r="T308">
-        <v>0.029</v>
+        <v>0.027</v>
       </c>
       <c r="U308">
-        <v>0.203</v>
+        <v>0.212</v>
       </c>
       <c r="V308">
         <v>0.125</v>
@@ -25956,7 +25956,7 @@
         <v>0.595</v>
       </c>
       <c r="X308">
-        <v>0.056</v>
+        <v>0.079</v>
       </c>
     </row>
     <row r="309" spans="1:24">
@@ -28741,7 +28741,7 @@
         <v>913</v>
       </c>
       <c r="O346">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P346">
         <v>130</v>
@@ -28753,22 +28753,22 @@
         <v>26</v>
       </c>
       <c r="S346">
-        <v>-14.6</v>
+        <v>-14.1</v>
       </c>
       <c r="T346">
-        <v>0.011</v>
+        <v>0.01</v>
       </c>
       <c r="U346">
-        <v>0.094</v>
+        <v>0.093</v>
       </c>
       <c r="V346">
-        <v>0.222</v>
+        <v>0.221</v>
       </c>
       <c r="W346">
-        <v>0.5570000000000001</v>
+        <v>0.552</v>
       </c>
       <c r="X346">
-        <v>0.159</v>
+        <v>0.156</v>
       </c>
     </row>
     <row r="347" spans="1:24">
@@ -31923,34 +31923,34 @@
         <v>900</v>
       </c>
       <c r="O389">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P389">
-        <v>311</v>
+        <v>325</v>
       </c>
       <c r="Q389">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="R389">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="S389">
-        <v>2</v>
+        <v>2.6</v>
       </c>
       <c r="T389">
         <v>0.028</v>
       </c>
       <c r="U389">
-        <v>0.139</v>
+        <v>0.137</v>
       </c>
       <c r="V389">
-        <v>0.182</v>
+        <v>0.183</v>
       </c>
       <c r="W389">
-        <v>0.583</v>
+        <v>0.591</v>
       </c>
       <c r="X389">
-        <v>0.171</v>
+        <v>0.173</v>
       </c>
     </row>
     <row r="390" spans="1:24">
@@ -33921,10 +33921,10 @@
         <v>901</v>
       </c>
       <c r="O416">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P416">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="Q416">
         <v>38</v>
@@ -33933,19 +33933,19 @@
         <v>27</v>
       </c>
       <c r="S416">
-        <v>5.9</v>
+        <v>5.5</v>
       </c>
       <c r="T416">
-        <v>0.034</v>
+        <v>0.033</v>
       </c>
       <c r="U416">
         <v>0.081</v>
       </c>
       <c r="V416">
-        <v>0.134</v>
+        <v>0.135</v>
       </c>
       <c r="W416">
-        <v>0.5629999999999999</v>
+        <v>0.5610000000000001</v>
       </c>
       <c r="X416">
         <v>0.121</v>
@@ -35993,34 +35993,34 @@
         <v>933</v>
       </c>
       <c r="O444">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P444">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="Q444">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R444">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="S444">
-        <v>0.5</v>
+        <v>1.2</v>
       </c>
       <c r="T444">
-        <v>0.066</v>
+        <v>0.06900000000000001</v>
       </c>
       <c r="U444">
-        <v>0.209</v>
+        <v>0.203</v>
       </c>
       <c r="V444">
         <v>0.177</v>
       </c>
       <c r="W444">
-        <v>0.706</v>
+        <v>0.705</v>
       </c>
       <c r="X444">
-        <v>0.063</v>
+        <v>0.07199999999999999</v>
       </c>
     </row>
     <row r="445" spans="1:24">
@@ -36659,34 +36659,34 @@
         <v>901</v>
       </c>
       <c r="O453">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P453">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="Q453">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R453">
         <v>6</v>
       </c>
       <c r="S453">
-        <v>-4.4</v>
+        <v>-2.1</v>
       </c>
       <c r="T453">
-        <v>0.045</v>
+        <v>0.043</v>
       </c>
       <c r="U453">
-        <v>0.115</v>
+        <v>0.127</v>
       </c>
       <c r="V453">
-        <v>0.163</v>
+        <v>0.171</v>
       </c>
       <c r="W453">
-        <v>0.508</v>
+        <v>0.5669999999999999</v>
       </c>
       <c r="X453">
-        <v>0.231</v>
+        <v>0.222</v>
       </c>
     </row>
     <row r="454" spans="1:24">
@@ -37103,34 +37103,34 @@
         <v>878</v>
       </c>
       <c r="O459">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P459">
-        <v>454</v>
+        <v>465</v>
       </c>
       <c r="Q459">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="R459">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="S459">
-        <v>-1.1</v>
+        <v>-1.7</v>
       </c>
       <c r="T459">
-        <v>0.025</v>
+        <v>0.028</v>
       </c>
       <c r="U459">
-        <v>0.067</v>
+        <v>0.066</v>
       </c>
       <c r="V459">
-        <v>0.227</v>
+        <v>0.226</v>
       </c>
       <c r="W459">
-        <v>0.491</v>
+        <v>0.494</v>
       </c>
       <c r="X459">
-        <v>0.219</v>
+        <v>0.215</v>
       </c>
     </row>
     <row r="460" spans="1:24">
@@ -37988,34 +37988,34 @@
         <v>886</v>
       </c>
       <c r="O471">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P471">
-        <v>426</v>
+        <v>446</v>
       </c>
       <c r="Q471">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="R471">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="S471">
-        <v>-2</v>
+        <v>-1.2</v>
       </c>
       <c r="T471">
         <v>0.023</v>
       </c>
       <c r="U471">
-        <v>0.114</v>
+        <v>0.113</v>
       </c>
       <c r="V471">
-        <v>0.196</v>
+        <v>0.197</v>
       </c>
       <c r="W471">
-        <v>0.513</v>
+        <v>0.518</v>
       </c>
       <c r="X471">
-        <v>0.152</v>
+        <v>0.154</v>
       </c>
     </row>
     <row r="472" spans="1:24">
@@ -38728,34 +38728,34 @@
         <v>881</v>
       </c>
       <c r="O481">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P481">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="Q481">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="R481">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="S481">
-        <v>5.1</v>
+        <v>3</v>
       </c>
       <c r="T481">
-        <v>0.031</v>
+        <v>0.03</v>
       </c>
       <c r="U481">
-        <v>0.08699999999999999</v>
+        <v>0.089</v>
       </c>
       <c r="V481">
-        <v>0.104</v>
+        <v>0.105</v>
       </c>
       <c r="W481">
-        <v>0.529</v>
+        <v>0.533</v>
       </c>
       <c r="X481">
-        <v>0.302</v>
+        <v>0.304</v>
       </c>
     </row>
     <row r="482" spans="1:24">
@@ -39838,31 +39838,31 @@
         <v>915</v>
       </c>
       <c r="O496">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P496">
-        <v>968</v>
+        <v>986</v>
       </c>
       <c r="Q496">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="R496">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="S496">
-        <v>-0.4</v>
+        <v>0</v>
       </c>
       <c r="T496">
         <v>0.008999999999999999</v>
       </c>
       <c r="U496">
-        <v>0.149</v>
+        <v>0.15</v>
       </c>
       <c r="V496">
-        <v>0.262</v>
+        <v>0.26</v>
       </c>
       <c r="W496">
-        <v>0.625</v>
+        <v>0.626</v>
       </c>
       <c r="X496">
         <v>0.238</v>
@@ -40504,19 +40504,19 @@
         <v>874</v>
       </c>
       <c r="O505">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="P505">
-        <v>859</v>
+        <v>880</v>
       </c>
       <c r="Q505">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="R505">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="S505">
-        <v>4.3</v>
+        <v>3.7</v>
       </c>
       <c r="T505">
         <v>0.054</v>
@@ -40525,10 +40525,10 @@
         <v>0.246</v>
       </c>
       <c r="V505">
-        <v>0.307</v>
+        <v>0.309</v>
       </c>
       <c r="W505">
-        <v>0.594</v>
+        <v>0.592</v>
       </c>
       <c r="X505">
         <v>0.192</v>
@@ -41318,34 +41318,34 @@
         <v>906</v>
       </c>
       <c r="O516">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P516">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="Q516">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="R516">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="S516">
-        <v>-7.6</v>
+        <v>-7.5</v>
       </c>
       <c r="T516">
-        <v>0.08</v>
+        <v>0.083</v>
       </c>
       <c r="U516">
         <v>0.144</v>
       </c>
       <c r="V516">
-        <v>0.172</v>
+        <v>0.169</v>
       </c>
       <c r="W516">
-        <v>0.555</v>
+        <v>0.5580000000000001</v>
       </c>
       <c r="X516">
-        <v>0.172</v>
+        <v>0.174</v>
       </c>
     </row>
     <row r="517" spans="1:24">

</xml_diff>

<commit_message>
This v2.2 will be SICK.
</commit_message>
<xml_diff>
--- a/Players_Data.xlsx
+++ b/Players_Data.xlsx
@@ -184,7 +184,7 @@
     <t>Ariel Hukporti</t>
   </si>
   <si>
-    <t>Armel Traore</t>
+    <t>Armel Traoré</t>
   </si>
   <si>
     <t>Ausar Thompson</t>
@@ -1216,7 +1216,7 @@
     <t>Mouhamed Gueye</t>
   </si>
   <si>
-    <t>Moussa Diabate</t>
+    <t>Moussa Diabaté</t>
   </si>
   <si>
     <t>Myles Turner</t>
@@ -1489,7 +1489,7 @@
     <t>Taylor Hendricks</t>
   </si>
   <si>
-    <t>Taze Moore</t>
+    <t>Tazé Moore</t>
   </si>
   <si>
     <t>Terance Mann</t>
@@ -1504,7 +1504,7 @@
     <t>Thomas Bryant</t>
   </si>
   <si>
-    <t>Tidjane Salaun</t>
+    <t>Tidjane Salaün</t>
   </si>
   <si>
     <t>Tim Hardaway Jr.</t>
@@ -25210,7 +25210,7 @@
         <v>3</v>
       </c>
       <c r="S298">
-        <v>11.5</v>
+        <v>11.4</v>
       </c>
       <c r="T298">
         <v>0.116</v>
@@ -25219,7 +25219,7 @@
         <v>0.147</v>
       </c>
       <c r="V298">
-        <v>0.108</v>
+        <v>0.107</v>
       </c>
       <c r="W298">
         <v>0.455</v>
@@ -33803,7 +33803,7 @@
         <v>0.057</v>
       </c>
       <c r="V414">
-        <v>0.147</v>
+        <v>0.149</v>
       </c>
       <c r="W414">
         <v>0.486</v>
@@ -39498,7 +39498,7 @@
         <v>0.112</v>
       </c>
       <c r="V491">
-        <v>0.227</v>
+        <v>0.226</v>
       </c>
       <c r="W491">
         <v>0.602</v>

</xml_diff>